<commit_message>
added Week 7 Tasks to Gantt chart
</commit_message>
<xml_diff>
--- a/docs/planningdocuments/gannt/GanttChart_POS_7.xlsx
+++ b/docs/planningdocuments/gannt/GanttChart_POS_7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\CPS353-POS\docs\planningdocuments\gannt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/CPS353-POS/docs/planningdocuments/gannt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7D7964-EC00-4B7D-B1C3-026CAFE988B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D43B1A7-DB77-AE4A-AC0F-726E9C1ECDDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="131">
   <si>
     <t>GANTT CHART</t>
   </si>
@@ -358,16 +358,10 @@
     <t xml:space="preserve">Database </t>
   </si>
   <si>
-    <t xml:space="preserve">Rental Checkout Customer Page </t>
-  </si>
-  <si>
     <t>Rental Check-in Employee Portal</t>
   </si>
   <si>
     <t xml:space="preserve">Admin Inventory Page </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Tables </t>
   </si>
   <si>
     <t>Upload to XAMMP</t>
@@ -503,6 +497,18 @@
   </si>
   <si>
     <t>Begin using HTTP Only Cookies in sessions</t>
+  </si>
+  <si>
+    <t>Rental Checkout Customer Page to Display DB Info</t>
+  </si>
+  <si>
+    <t>Meet with Christina to Finalize Users Tables and upload to XAMMP</t>
+  </si>
+  <si>
+    <t>Product Tables with Data</t>
+  </si>
+  <si>
+    <t>Work with Olamide to get Add to cart button functioning on Rental page</t>
   </si>
 </sst>
 </file>
@@ -728,7 +734,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -877,6 +883,18 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFCE4D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1060,7 +1078,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1431,6 +1449,70 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="25" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="24" fillId="25" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="24" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1445,14 +1527,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1463,63 +1540,13 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="25" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="24" fillId="25" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="24" fillId="18" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1840,24 +1867,25 @@
     <tabColor rgb="FF3D85C6"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BZ104"/>
+  <dimension ref="A1:BZ107"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM47" sqref="AM47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A56" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="48.88671875" customWidth="1"/>
+    <col min="3" max="3" width="62" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
     <col min="5" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" customWidth="1"/>
-    <col min="9" max="78" width="3.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" customWidth="1"/>
+    <col min="9" max="78" width="3.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -1937,40 +1965,40 @@
       <c r="BY1" s="1"/>
       <c r="BZ1" s="1"/>
     </row>
-    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="136" t="s">
+      <c r="B2" s="162" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="163"/>
+      <c r="E2" s="163"/>
+      <c r="F2" s="163"/>
+      <c r="G2" s="163"/>
       <c r="H2" s="10"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="137"/>
-      <c r="L2" s="137"/>
-      <c r="M2" s="137"/>
-      <c r="N2" s="137"/>
-      <c r="O2" s="139"/>
-      <c r="P2" s="137"/>
-      <c r="Q2" s="137"/>
-      <c r="R2" s="137"/>
-      <c r="S2" s="137"/>
-      <c r="T2" s="137"/>
-      <c r="U2" s="137"/>
-      <c r="V2" s="137"/>
-      <c r="W2" s="137"/>
-      <c r="X2" s="137"/>
-      <c r="Y2" s="137"/>
-      <c r="Z2" s="137"/>
-      <c r="AA2" s="137"/>
-      <c r="AB2" s="137"/>
-      <c r="AC2" s="137"/>
-      <c r="AD2" s="137"/>
-      <c r="AE2" s="137"/>
+      <c r="I2" s="164"/>
+      <c r="J2" s="163"/>
+      <c r="K2" s="163"/>
+      <c r="L2" s="163"/>
+      <c r="M2" s="163"/>
+      <c r="N2" s="163"/>
+      <c r="O2" s="165"/>
+      <c r="P2" s="163"/>
+      <c r="Q2" s="163"/>
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="163"/>
+      <c r="U2" s="163"/>
+      <c r="V2" s="163"/>
+      <c r="W2" s="163"/>
+      <c r="X2" s="163"/>
+      <c r="Y2" s="163"/>
+      <c r="Z2" s="163"/>
+      <c r="AA2" s="163"/>
+      <c r="AB2" s="163"/>
+      <c r="AC2" s="163"/>
+      <c r="AD2" s="163"/>
+      <c r="AE2" s="163"/>
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
       <c r="AH2" s="11"/>
@@ -2019,7 +2047,7 @@
       <c r="BY2" s="1"/>
       <c r="BZ2" s="1"/>
     </row>
-    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
@@ -2099,43 +2127,43 @@
       <c r="BY3" s="1"/>
       <c r="BZ3" s="1"/>
     </row>
-    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="155" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="141"/>
-      <c r="D4" s="142" t="s">
+      <c r="C4" s="156"/>
+      <c r="D4" s="166" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="143"/>
-      <c r="F4" s="143"/>
-      <c r="G4" s="143"/>
+      <c r="E4" s="158"/>
+      <c r="F4" s="158"/>
+      <c r="G4" s="158"/>
       <c r="H4" s="16"/>
-      <c r="I4" s="140" t="s">
+      <c r="I4" s="155" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="141"/>
-      <c r="K4" s="141"/>
-      <c r="L4" s="141"/>
-      <c r="M4" s="141"/>
-      <c r="N4" s="141"/>
-      <c r="O4" s="141"/>
-      <c r="P4" s="144" t="s">
+      <c r="J4" s="156"/>
+      <c r="K4" s="156"/>
+      <c r="L4" s="156"/>
+      <c r="M4" s="156"/>
+      <c r="N4" s="156"/>
+      <c r="O4" s="156"/>
+      <c r="P4" s="167" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="143"/>
-      <c r="R4" s="143"/>
-      <c r="S4" s="143"/>
-      <c r="T4" s="143"/>
-      <c r="U4" s="143"/>
-      <c r="V4" s="143"/>
-      <c r="W4" s="143"/>
-      <c r="X4" s="143"/>
-      <c r="Y4" s="143"/>
-      <c r="Z4" s="143"/>
-      <c r="AA4" s="143"/>
-      <c r="AB4" s="143"/>
+      <c r="Q4" s="158"/>
+      <c r="R4" s="158"/>
+      <c r="S4" s="158"/>
+      <c r="T4" s="158"/>
+      <c r="U4" s="158"/>
+      <c r="V4" s="158"/>
+      <c r="W4" s="158"/>
+      <c r="X4" s="158"/>
+      <c r="Y4" s="158"/>
+      <c r="Z4" s="158"/>
+      <c r="AA4" s="158"/>
+      <c r="AB4" s="158"/>
       <c r="AC4" s="17"/>
       <c r="AD4" s="9"/>
       <c r="AE4" s="9"/>
@@ -2187,42 +2215,42 @@
       <c r="BY4" s="1"/>
       <c r="BZ4" s="1"/>
     </row>
-    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="140" t="s">
+      <c r="B5" s="155" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="141"/>
-      <c r="D5" s="154" t="s">
+      <c r="C5" s="156"/>
+      <c r="D5" s="157" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="143"/>
-      <c r="F5" s="143"/>
-      <c r="G5" s="143"/>
+      <c r="E5" s="158"/>
+      <c r="F5" s="158"/>
+      <c r="G5" s="158"/>
       <c r="H5" s="18"/>
-      <c r="I5" s="140" t="s">
+      <c r="I5" s="155" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="141"/>
-      <c r="K5" s="141"/>
-      <c r="L5" s="141"/>
-      <c r="M5" s="141"/>
-      <c r="N5" s="141"/>
-      <c r="O5" s="141"/>
-      <c r="P5" s="155">
+      <c r="J5" s="156"/>
+      <c r="K5" s="156"/>
+      <c r="L5" s="156"/>
+      <c r="M5" s="156"/>
+      <c r="N5" s="156"/>
+      <c r="O5" s="156"/>
+      <c r="P5" s="159">
         <v>44846</v>
       </c>
-      <c r="Q5" s="143"/>
-      <c r="R5" s="143"/>
-      <c r="S5" s="143"/>
-      <c r="T5" s="143"/>
-      <c r="U5" s="143"/>
-      <c r="V5" s="143"/>
-      <c r="W5" s="143"/>
-      <c r="X5" s="143"/>
-      <c r="Y5" s="143"/>
-      <c r="Z5" s="143"/>
-      <c r="AA5" s="143"/>
+      <c r="Q5" s="158"/>
+      <c r="R5" s="158"/>
+      <c r="S5" s="158"/>
+      <c r="T5" s="158"/>
+      <c r="U5" s="158"/>
+      <c r="V5" s="158"/>
+      <c r="W5" s="158"/>
+      <c r="X5" s="158"/>
+      <c r="Y5" s="158"/>
+      <c r="Z5" s="158"/>
+      <c r="AA5" s="158"/>
       <c r="AB5" s="19"/>
       <c r="AC5" s="17"/>
       <c r="AD5" s="1"/>
@@ -2275,7 +2303,7 @@
       <c r="BY5" s="1"/>
       <c r="BZ5" s="1"/>
     </row>
-    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="21"/>
       <c r="B6" s="48" t="s">
         <v>49</v>
@@ -2359,7 +2387,7 @@
       <c r="BY6" s="21"/>
       <c r="BZ6" s="21"/>
     </row>
-    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="21"/>
       <c r="B7" s="22" t="s">
         <v>50</v>
@@ -2443,7 +2471,7 @@
       <c r="BY7" s="21"/>
       <c r="BZ7" s="21"/>
     </row>
-    <row r="8" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="21"/>
       <c r="B8" s="22"/>
       <c r="C8" s="22"/>
@@ -2523,209 +2551,209 @@
       <c r="BY8" s="21"/>
       <c r="BZ8" s="21"/>
     </row>
-    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="24"/>
-      <c r="B9" s="134" t="s">
+      <c r="B9" s="160" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="134" t="s">
+      <c r="C9" s="160" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="134" t="s">
+      <c r="D9" s="160" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="134" t="s">
+      <c r="E9" s="160" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="134" t="s">
+      <c r="F9" s="160" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="134" t="s">
+      <c r="G9" s="160" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="145" t="s">
+      <c r="H9" s="168" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="147"/>
-      <c r="J9" s="148"/>
-      <c r="K9" s="148"/>
-      <c r="L9" s="148"/>
-      <c r="M9" s="148"/>
-      <c r="N9" s="148"/>
-      <c r="O9" s="148"/>
-      <c r="P9" s="148"/>
-      <c r="Q9" s="148"/>
-      <c r="R9" s="148"/>
-      <c r="S9" s="148"/>
-      <c r="T9" s="148"/>
-      <c r="U9" s="148"/>
-      <c r="V9" s="148"/>
-      <c r="W9" s="148"/>
+      <c r="I9" s="170"/>
+      <c r="J9" s="150"/>
+      <c r="K9" s="150"/>
+      <c r="L9" s="150"/>
+      <c r="M9" s="150"/>
+      <c r="N9" s="150"/>
+      <c r="O9" s="150"/>
+      <c r="P9" s="150"/>
+      <c r="Q9" s="150"/>
+      <c r="R9" s="150"/>
+      <c r="S9" s="150"/>
+      <c r="T9" s="150"/>
+      <c r="U9" s="150"/>
+      <c r="V9" s="150"/>
+      <c r="W9" s="150"/>
       <c r="X9" s="149"/>
-      <c r="Y9" s="148"/>
-      <c r="Z9" s="148"/>
-      <c r="AA9" s="148"/>
-      <c r="AB9" s="148"/>
-      <c r="AC9" s="148"/>
-      <c r="AD9" s="148"/>
-      <c r="AE9" s="148"/>
-      <c r="AF9" s="148"/>
-      <c r="AG9" s="148"/>
-      <c r="AH9" s="148"/>
-      <c r="AI9" s="148"/>
-      <c r="AJ9" s="148"/>
-      <c r="AK9" s="148"/>
-      <c r="AL9" s="148"/>
+      <c r="Y9" s="150"/>
+      <c r="Z9" s="150"/>
+      <c r="AA9" s="150"/>
+      <c r="AB9" s="150"/>
+      <c r="AC9" s="150"/>
+      <c r="AD9" s="150"/>
+      <c r="AE9" s="150"/>
+      <c r="AF9" s="150"/>
+      <c r="AG9" s="150"/>
+      <c r="AH9" s="150"/>
+      <c r="AI9" s="150"/>
+      <c r="AJ9" s="150"/>
+      <c r="AK9" s="150"/>
+      <c r="AL9" s="150"/>
       <c r="AM9" s="149"/>
-      <c r="AN9" s="148"/>
-      <c r="AO9" s="148"/>
-      <c r="AP9" s="148"/>
-      <c r="AQ9" s="148"/>
-      <c r="AR9" s="148"/>
-      <c r="AS9" s="148"/>
-      <c r="AT9" s="148"/>
-      <c r="AU9" s="148"/>
-      <c r="AV9" s="148"/>
-      <c r="AW9" s="148"/>
-      <c r="AX9" s="148"/>
-      <c r="AY9" s="148"/>
-      <c r="AZ9" s="148"/>
-      <c r="BA9" s="148"/>
+      <c r="AN9" s="150"/>
+      <c r="AO9" s="150"/>
+      <c r="AP9" s="150"/>
+      <c r="AQ9" s="150"/>
+      <c r="AR9" s="150"/>
+      <c r="AS9" s="150"/>
+      <c r="AT9" s="150"/>
+      <c r="AU9" s="150"/>
+      <c r="AV9" s="150"/>
+      <c r="AW9" s="150"/>
+      <c r="AX9" s="150"/>
+      <c r="AY9" s="150"/>
+      <c r="AZ9" s="150"/>
+      <c r="BA9" s="150"/>
       <c r="BB9" s="149"/>
-      <c r="BC9" s="148"/>
-      <c r="BD9" s="148"/>
-      <c r="BE9" s="148"/>
-      <c r="BF9" s="148"/>
-      <c r="BG9" s="148"/>
-      <c r="BH9" s="148"/>
-      <c r="BI9" s="148"/>
-      <c r="BJ9" s="148"/>
-      <c r="BK9" s="148"/>
-      <c r="BL9" s="148"/>
-      <c r="BM9" s="148"/>
-      <c r="BN9" s="148"/>
-      <c r="BO9" s="148"/>
-      <c r="BP9" s="148"/>
-      <c r="BQ9" s="148"/>
-      <c r="BR9" s="148"/>
-      <c r="BS9" s="148"/>
-      <c r="BT9" s="148"/>
-      <c r="BU9" s="148"/>
-      <c r="BV9" s="148"/>
-      <c r="BW9" s="148"/>
-      <c r="BX9" s="148"/>
-      <c r="BY9" s="148"/>
-      <c r="BZ9" s="153"/>
+      <c r="BC9" s="150"/>
+      <c r="BD9" s="150"/>
+      <c r="BE9" s="150"/>
+      <c r="BF9" s="150"/>
+      <c r="BG9" s="150"/>
+      <c r="BH9" s="150"/>
+      <c r="BI9" s="150"/>
+      <c r="BJ9" s="150"/>
+      <c r="BK9" s="150"/>
+      <c r="BL9" s="150"/>
+      <c r="BM9" s="150"/>
+      <c r="BN9" s="150"/>
+      <c r="BO9" s="150"/>
+      <c r="BP9" s="150"/>
+      <c r="BQ9" s="150"/>
+      <c r="BR9" s="150"/>
+      <c r="BS9" s="150"/>
+      <c r="BT9" s="150"/>
+      <c r="BU9" s="150"/>
+      <c r="BV9" s="150"/>
+      <c r="BW9" s="150"/>
+      <c r="BX9" s="150"/>
+      <c r="BY9" s="150"/>
+      <c r="BZ9" s="151"/>
     </row>
-    <row r="10" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:78" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="25"/>
-      <c r="B10" s="135"/>
-      <c r="C10" s="135"/>
-      <c r="D10" s="135"/>
-      <c r="E10" s="135"/>
-      <c r="F10" s="135"/>
-      <c r="G10" s="135"/>
-      <c r="H10" s="146"/>
-      <c r="I10" s="150" t="s">
+      <c r="B10" s="161"/>
+      <c r="C10" s="161"/>
+      <c r="D10" s="161"/>
+      <c r="E10" s="161"/>
+      <c r="F10" s="161"/>
+      <c r="G10" s="161"/>
+      <c r="H10" s="169"/>
+      <c r="I10" s="152" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10" s="153"/>
+      <c r="K10" s="153"/>
+      <c r="L10" s="153"/>
+      <c r="M10" s="154"/>
+      <c r="N10" s="152" t="s">
+        <v>101</v>
+      </c>
+      <c r="O10" s="153"/>
+      <c r="P10" s="153"/>
+      <c r="Q10" s="153"/>
+      <c r="R10" s="154"/>
+      <c r="S10" s="152" t="s">
         <v>102</v>
       </c>
-      <c r="J10" s="151"/>
-      <c r="K10" s="151"/>
-      <c r="L10" s="151"/>
-      <c r="M10" s="152"/>
-      <c r="N10" s="150" t="s">
-        <v>103</v>
-      </c>
-      <c r="O10" s="151"/>
-      <c r="P10" s="151"/>
-      <c r="Q10" s="151"/>
-      <c r="R10" s="152"/>
-      <c r="S10" s="150" t="s">
-        <v>104</v>
-      </c>
-      <c r="T10" s="151"/>
-      <c r="U10" s="151"/>
-      <c r="V10" s="151"/>
-      <c r="W10" s="152"/>
-      <c r="X10" s="150" t="s">
+      <c r="T10" s="153"/>
+      <c r="U10" s="153"/>
+      <c r="V10" s="153"/>
+      <c r="W10" s="154"/>
+      <c r="X10" s="152" t="s">
+        <v>108</v>
+      </c>
+      <c r="Y10" s="153"/>
+      <c r="Z10" s="153"/>
+      <c r="AA10" s="153"/>
+      <c r="AB10" s="154"/>
+      <c r="AC10" s="152" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD10" s="153"/>
+      <c r="AE10" s="153"/>
+      <c r="AF10" s="153"/>
+      <c r="AG10" s="154"/>
+      <c r="AH10" s="152" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI10" s="153"/>
+      <c r="AJ10" s="153"/>
+      <c r="AK10" s="153"/>
+      <c r="AL10" s="154"/>
+      <c r="AM10" s="152" t="s">
         <v>110</v>
       </c>
-      <c r="Y10" s="151"/>
-      <c r="Z10" s="151"/>
-      <c r="AA10" s="151"/>
-      <c r="AB10" s="152"/>
-      <c r="AC10" s="150" t="s">
+      <c r="AN10" s="153"/>
+      <c r="AO10" s="153"/>
+      <c r="AP10" s="153"/>
+      <c r="AQ10" s="154"/>
+      <c r="AR10" s="152" t="s">
         <v>111</v>
       </c>
-      <c r="AD10" s="151"/>
-      <c r="AE10" s="151"/>
-      <c r="AF10" s="151"/>
-      <c r="AG10" s="152"/>
-      <c r="AH10" s="150" t="s">
-        <v>86</v>
-      </c>
-      <c r="AI10" s="151"/>
-      <c r="AJ10" s="151"/>
-      <c r="AK10" s="151"/>
-      <c r="AL10" s="152"/>
-      <c r="AM10" s="150" t="s">
+      <c r="AS10" s="153"/>
+      <c r="AT10" s="153"/>
+      <c r="AU10" s="153"/>
+      <c r="AV10" s="154"/>
+      <c r="AW10" s="152" t="s">
         <v>112</v>
       </c>
-      <c r="AN10" s="151"/>
-      <c r="AO10" s="151"/>
-      <c r="AP10" s="151"/>
-      <c r="AQ10" s="152"/>
-      <c r="AR10" s="150" t="s">
-        <v>113</v>
-      </c>
-      <c r="AS10" s="151"/>
-      <c r="AT10" s="151"/>
-      <c r="AU10" s="151"/>
-      <c r="AV10" s="152"/>
-      <c r="AW10" s="150" t="s">
-        <v>114</v>
-      </c>
-      <c r="AX10" s="151"/>
-      <c r="AY10" s="151"/>
-      <c r="AZ10" s="151"/>
-      <c r="BA10" s="152"/>
-      <c r="BB10" s="150" t="s">
+      <c r="AX10" s="153"/>
+      <c r="AY10" s="153"/>
+      <c r="AZ10" s="153"/>
+      <c r="BA10" s="154"/>
+      <c r="BB10" s="152" t="s">
         <v>12</v>
       </c>
-      <c r="BC10" s="151"/>
-      <c r="BD10" s="151"/>
-      <c r="BE10" s="151"/>
-      <c r="BF10" s="152"/>
-      <c r="BG10" s="150" t="s">
+      <c r="BC10" s="153"/>
+      <c r="BD10" s="153"/>
+      <c r="BE10" s="153"/>
+      <c r="BF10" s="154"/>
+      <c r="BG10" s="152" t="s">
         <v>13</v>
       </c>
-      <c r="BH10" s="151"/>
-      <c r="BI10" s="151"/>
-      <c r="BJ10" s="151"/>
-      <c r="BK10" s="152"/>
-      <c r="BL10" s="150" t="s">
+      <c r="BH10" s="153"/>
+      <c r="BI10" s="153"/>
+      <c r="BJ10" s="153"/>
+      <c r="BK10" s="154"/>
+      <c r="BL10" s="152" t="s">
         <v>14</v>
       </c>
-      <c r="BM10" s="151"/>
-      <c r="BN10" s="151"/>
-      <c r="BO10" s="151"/>
-      <c r="BP10" s="152"/>
-      <c r="BQ10" s="150" t="s">
+      <c r="BM10" s="153"/>
+      <c r="BN10" s="153"/>
+      <c r="BO10" s="153"/>
+      <c r="BP10" s="154"/>
+      <c r="BQ10" s="152" t="s">
         <v>15</v>
       </c>
-      <c r="BR10" s="151"/>
-      <c r="BS10" s="151"/>
-      <c r="BT10" s="151"/>
-      <c r="BU10" s="152"/>
-      <c r="BV10" s="150" t="s">
+      <c r="BR10" s="153"/>
+      <c r="BS10" s="153"/>
+      <c r="BT10" s="153"/>
+      <c r="BU10" s="154"/>
+      <c r="BV10" s="152" t="s">
         <v>16</v>
       </c>
-      <c r="BW10" s="151"/>
-      <c r="BX10" s="151"/>
-      <c r="BY10" s="151"/>
-      <c r="BZ10" s="152"/>
+      <c r="BW10" s="153"/>
+      <c r="BX10" s="153"/>
+      <c r="BY10" s="153"/>
+      <c r="BZ10" s="154"/>
     </row>
-    <row r="11" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="21"/>
       <c r="B11" s="26">
         <v>1</v>
@@ -2739,217 +2767,217 @@
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
       <c r="I11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="K11" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="J11" s="30" t="s">
+      <c r="L11" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="K11" s="31" t="s">
+      <c r="M11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="L11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="M11" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="N11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="O11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="P11" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="O11" s="30" t="s">
+      <c r="Q11" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="P11" s="31" t="s">
+      <c r="R11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="Q11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="R11" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="S11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="T11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="U11" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="T11" s="30" t="s">
+      <c r="V11" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="U11" s="31" t="s">
+      <c r="W11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="V11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="W11" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="X11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z11" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="Y11" s="30" t="s">
+      <c r="AA11" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="Z11" s="31" t="s">
+      <c r="AB11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="AA11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="AB11" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="AC11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="AD11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="AE11" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="AD11" s="30" t="s">
+      <c r="AF11" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="AE11" s="31" t="s">
+      <c r="AG11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="AF11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="AG11" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="AH11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="AJ11" s="126" t="s">
         <v>105</v>
       </c>
-      <c r="AI11" s="30" t="s">
+      <c r="AK11" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="AJ11" s="126" t="s">
+      <c r="AL11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="AK11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="AL11" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="AM11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="AN11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="AO11" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="AN11" s="30" t="s">
+      <c r="AP11" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="AO11" s="31" t="s">
+      <c r="AQ11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="AP11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="AQ11" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="AR11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="AT11" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="AS11" s="30" t="s">
+      <c r="AU11" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="AT11" s="31" t="s">
+      <c r="AV11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="AU11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="AV11" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="AW11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY11" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="AX11" s="30" t="s">
+      <c r="AZ11" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="AY11" s="31" t="s">
+      <c r="BA11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="AZ11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="BA11" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="BB11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="BC11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="BD11" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="BC11" s="30" t="s">
+      <c r="BE11" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="BD11" s="31" t="s">
+      <c r="BF11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="BE11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="BF11" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="BG11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="BH11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="BI11" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="BH11" s="30" t="s">
+      <c r="BJ11" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="BI11" s="31" t="s">
+      <c r="BK11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="BJ11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="BK11" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="BL11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="BM11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="BN11" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="BM11" s="30" t="s">
+      <c r="BO11" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="BN11" s="31" t="s">
+      <c r="BP11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="BO11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="BP11" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="BQ11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="BR11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="BS11" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="BR11" s="30" t="s">
+      <c r="BT11" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="BS11" s="31" t="s">
+      <c r="BU11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="BT11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="BU11" s="29" t="s">
-        <v>109</v>
-      </c>
       <c r="BV11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="BW11" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="BX11" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="BW11" s="30" t="s">
+      <c r="BY11" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="BX11" s="31" t="s">
+      <c r="BZ11" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="BY11" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="BZ11" s="29" t="s">
-        <v>109</v>
-      </c>
     </row>
-    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A12" s="32"/>
       <c r="B12" s="33">
         <v>1.1000000000000001</v>
@@ -2993,11 +3021,11 @@
       <c r="Z12" s="38"/>
       <c r="AA12" s="38"/>
       <c r="AB12" s="38"/>
-      <c r="AC12" s="38"/>
-      <c r="AD12" s="38"/>
-      <c r="AE12" s="38"/>
-      <c r="AF12" s="38"/>
-      <c r="AG12" s="38"/>
+      <c r="AC12" s="173"/>
+      <c r="AD12" s="173"/>
+      <c r="AE12" s="173"/>
+      <c r="AF12" s="173"/>
+      <c r="AG12" s="173"/>
       <c r="AH12" s="38"/>
       <c r="AI12" s="38"/>
       <c r="AJ12" s="38"/>
@@ -3044,7 +3072,7 @@
       <c r="BY12" s="38"/>
       <c r="BZ12" s="38"/>
     </row>
-    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A13" s="32"/>
       <c r="B13" s="33" t="s">
         <v>17</v>
@@ -3088,11 +3116,11 @@
       <c r="Z13" s="38"/>
       <c r="AA13" s="38"/>
       <c r="AB13" s="38"/>
-      <c r="AC13" s="38"/>
-      <c r="AD13" s="38"/>
-      <c r="AE13" s="38"/>
-      <c r="AF13" s="38"/>
-      <c r="AG13" s="38"/>
+      <c r="AC13" s="173"/>
+      <c r="AD13" s="173"/>
+      <c r="AE13" s="173"/>
+      <c r="AF13" s="173"/>
+      <c r="AG13" s="173"/>
       <c r="AH13" s="38"/>
       <c r="AI13" s="38"/>
       <c r="AJ13" s="38"/>
@@ -3139,7 +3167,7 @@
       <c r="BY13" s="38"/>
       <c r="BZ13" s="38"/>
     </row>
-    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A14" s="32"/>
       <c r="B14" s="33">
         <v>1.2</v>
@@ -3183,11 +3211,11 @@
       <c r="Z14" s="38"/>
       <c r="AA14" s="38"/>
       <c r="AB14" s="38"/>
-      <c r="AC14" s="38"/>
-      <c r="AD14" s="38"/>
-      <c r="AE14" s="38"/>
-      <c r="AF14" s="38"/>
-      <c r="AG14" s="38"/>
+      <c r="AC14" s="173"/>
+      <c r="AD14" s="173"/>
+      <c r="AE14" s="173"/>
+      <c r="AF14" s="173"/>
+      <c r="AG14" s="173"/>
       <c r="AH14" s="38"/>
       <c r="AI14" s="38"/>
       <c r="AJ14" s="38"/>
@@ -3234,7 +3262,7 @@
       <c r="BY14" s="38"/>
       <c r="BZ14" s="38"/>
     </row>
-    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A15" s="32"/>
       <c r="B15" s="33">
         <v>1.3</v>
@@ -3278,11 +3306,11 @@
       <c r="Z15" s="38"/>
       <c r="AA15" s="38"/>
       <c r="AB15" s="38"/>
-      <c r="AC15" s="38"/>
-      <c r="AD15" s="38"/>
-      <c r="AE15" s="38"/>
-      <c r="AF15" s="38"/>
-      <c r="AG15" s="38"/>
+      <c r="AC15" s="173"/>
+      <c r="AD15" s="173"/>
+      <c r="AE15" s="173"/>
+      <c r="AF15" s="173"/>
+      <c r="AG15" s="173"/>
       <c r="AH15" s="38"/>
       <c r="AI15" s="38"/>
       <c r="AJ15" s="38"/>
@@ -3329,7 +3357,7 @@
       <c r="BY15" s="38"/>
       <c r="BZ15" s="38"/>
     </row>
-    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A16" s="32"/>
       <c r="B16" s="33">
         <v>1.4</v>
@@ -3373,11 +3401,11 @@
       <c r="Z16" s="38"/>
       <c r="AA16" s="38"/>
       <c r="AB16" s="38"/>
-      <c r="AC16" s="38"/>
-      <c r="AD16" s="38"/>
-      <c r="AE16" s="38"/>
-      <c r="AF16" s="38"/>
-      <c r="AG16" s="38"/>
+      <c r="AC16" s="173"/>
+      <c r="AD16" s="173"/>
+      <c r="AE16" s="173"/>
+      <c r="AF16" s="173"/>
+      <c r="AG16" s="173"/>
       <c r="AH16" s="38"/>
       <c r="AI16" s="38"/>
       <c r="AJ16" s="38"/>
@@ -3424,7 +3452,7 @@
       <c r="BY16" s="38"/>
       <c r="BZ16" s="38"/>
     </row>
-    <row r="17" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A17" s="32"/>
       <c r="B17" s="33">
         <v>1.5</v>
@@ -3468,11 +3496,11 @@
       <c r="Z17" s="38"/>
       <c r="AA17" s="38"/>
       <c r="AB17" s="38"/>
-      <c r="AC17" s="38"/>
-      <c r="AD17" s="38"/>
-      <c r="AE17" s="38"/>
-      <c r="AF17" s="38"/>
-      <c r="AG17" s="38"/>
+      <c r="AC17" s="173"/>
+      <c r="AD17" s="173"/>
+      <c r="AE17" s="173"/>
+      <c r="AF17" s="173"/>
+      <c r="AG17" s="173"/>
       <c r="AH17" s="38"/>
       <c r="AI17" s="38"/>
       <c r="AJ17" s="38"/>
@@ -3519,7 +3547,7 @@
       <c r="BY17" s="38"/>
       <c r="BZ17" s="38"/>
     </row>
-    <row r="18" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A18" s="32"/>
       <c r="B18" s="33">
         <v>1.6</v>
@@ -3563,11 +3591,11 @@
       <c r="Z18" s="38"/>
       <c r="AA18" s="38"/>
       <c r="AB18" s="38"/>
-      <c r="AC18" s="38"/>
-      <c r="AD18" s="38"/>
-      <c r="AE18" s="38"/>
-      <c r="AF18" s="38"/>
-      <c r="AG18" s="38"/>
+      <c r="AC18" s="173"/>
+      <c r="AD18" s="173"/>
+      <c r="AE18" s="173"/>
+      <c r="AF18" s="173"/>
+      <c r="AG18" s="173"/>
       <c r="AH18" s="38"/>
       <c r="AI18" s="38"/>
       <c r="AJ18" s="38"/>
@@ -3614,7 +3642,7 @@
       <c r="BY18" s="38"/>
       <c r="BZ18" s="38"/>
     </row>
-    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A19" s="32"/>
       <c r="B19" s="33">
         <v>1.7</v>
@@ -3658,11 +3686,11 @@
       <c r="Z19" s="38"/>
       <c r="AA19" s="38"/>
       <c r="AB19" s="38"/>
-      <c r="AC19" s="38"/>
-      <c r="AD19" s="38"/>
-      <c r="AE19" s="38"/>
-      <c r="AF19" s="38"/>
-      <c r="AG19" s="38"/>
+      <c r="AC19" s="173"/>
+      <c r="AD19" s="173"/>
+      <c r="AE19" s="173"/>
+      <c r="AF19" s="173"/>
+      <c r="AG19" s="173"/>
       <c r="AH19" s="38"/>
       <c r="AI19" s="38"/>
       <c r="AJ19" s="38"/>
@@ -3709,7 +3737,7 @@
       <c r="BY19" s="38"/>
       <c r="BZ19" s="38"/>
     </row>
-    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A20" s="32"/>
       <c r="B20" s="33"/>
       <c r="C20" s="34"/>
@@ -3738,11 +3766,11 @@
       <c r="Z20" s="38"/>
       <c r="AA20" s="38"/>
       <c r="AB20" s="38"/>
-      <c r="AC20" s="38"/>
-      <c r="AD20" s="38"/>
-      <c r="AE20" s="38"/>
-      <c r="AF20" s="38"/>
-      <c r="AG20" s="38"/>
+      <c r="AC20" s="173"/>
+      <c r="AD20" s="173"/>
+      <c r="AE20" s="173"/>
+      <c r="AF20" s="173"/>
+      <c r="AG20" s="173"/>
       <c r="AH20" s="38"/>
       <c r="AI20" s="38"/>
       <c r="AJ20" s="38"/>
@@ -3789,7 +3817,7 @@
       <c r="BY20" s="38"/>
       <c r="BZ20" s="38"/>
     </row>
-    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A21" s="32"/>
       <c r="B21" s="33"/>
       <c r="C21" s="34"/>
@@ -3818,11 +3846,11 @@
       <c r="Z21" s="38"/>
       <c r="AA21" s="38"/>
       <c r="AB21" s="38"/>
-      <c r="AC21" s="38"/>
-      <c r="AD21" s="38"/>
-      <c r="AE21" s="38"/>
-      <c r="AF21" s="38"/>
-      <c r="AG21" s="38"/>
+      <c r="AC21" s="173"/>
+      <c r="AD21" s="173"/>
+      <c r="AE21" s="173"/>
+      <c r="AF21" s="173"/>
+      <c r="AG21" s="173"/>
       <c r="AH21" s="38"/>
       <c r="AI21" s="38"/>
       <c r="AJ21" s="38"/>
@@ -3869,7 +3897,7 @@
       <c r="BY21" s="38"/>
       <c r="BZ21" s="38"/>
     </row>
-    <row r="22" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="21"/>
       <c r="B22" s="26">
         <v>2</v>
@@ -3953,7 +3981,7 @@
       <c r="BY22" s="29"/>
       <c r="BZ22" s="29"/>
     </row>
-    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A23" s="32"/>
       <c r="B23" s="33">
         <v>2.1</v>
@@ -4043,7 +4071,7 @@
       <c r="BY23" s="38"/>
       <c r="BZ23" s="38"/>
     </row>
-    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A24" s="32"/>
       <c r="B24" s="33">
         <v>2.2000000000000002</v>
@@ -4134,7 +4162,7 @@
       <c r="BY24" s="38"/>
       <c r="BZ24" s="38"/>
     </row>
-    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A25" s="32"/>
       <c r="B25" s="33">
         <v>2.2999999999999998</v>
@@ -4225,7 +4253,7 @@
       <c r="BY25" s="38"/>
       <c r="BZ25" s="38"/>
     </row>
-    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A26" s="32"/>
       <c r="B26" s="33" t="s">
         <v>18</v>
@@ -4315,7 +4343,7 @@
       <c r="BY26" s="38"/>
       <c r="BZ26" s="38"/>
     </row>
-    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A27" s="32"/>
       <c r="B27" s="33">
         <v>2.4</v>
@@ -4406,7 +4434,7 @@
       <c r="BY27" s="38"/>
       <c r="BZ27" s="38"/>
     </row>
-    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A28" s="32"/>
       <c r="B28" s="33">
         <v>2.5</v>
@@ -4497,7 +4525,7 @@
       <c r="BY28" s="38"/>
       <c r="BZ28" s="38"/>
     </row>
-    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A29" s="32"/>
       <c r="B29" s="33">
         <v>2.6</v>
@@ -4587,7 +4615,7 @@
       <c r="BY29" s="38"/>
       <c r="BZ29" s="38"/>
     </row>
-    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A30" s="32"/>
       <c r="B30" s="33">
         <v>2.7</v>
@@ -4678,7 +4706,7 @@
       <c r="BY30" s="38"/>
       <c r="BZ30" s="38"/>
     </row>
-    <row r="31" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A31" s="32"/>
       <c r="B31" s="33">
         <v>2.8</v>
@@ -4769,7 +4797,7 @@
       <c r="BY31" s="38"/>
       <c r="BZ31" s="38"/>
     </row>
-    <row r="32" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A32" s="32"/>
       <c r="B32" s="33">
         <v>2.9</v>
@@ -4859,7 +4887,7 @@
       <c r="BY32" s="38"/>
       <c r="BZ32" s="38"/>
     </row>
-    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A33" s="32"/>
       <c r="B33" s="46">
         <v>2.1</v>
@@ -4949,7 +4977,7 @@
       <c r="BY33" s="38"/>
       <c r="BZ33" s="38"/>
     </row>
-    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A34" s="32"/>
       <c r="B34" s="46">
         <v>2.11</v>
@@ -5031,7 +5059,7 @@
       <c r="BY34" s="38"/>
       <c r="BZ34" s="38"/>
     </row>
-    <row r="35" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="21"/>
       <c r="B35" s="26">
         <v>3</v>
@@ -5115,7 +5143,7 @@
       <c r="BY35" s="29"/>
       <c r="BZ35" s="29"/>
     </row>
-    <row r="36" spans="1:78" s="75" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:78" s="75" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="78"/>
       <c r="B36" s="79"/>
       <c r="C36" s="80" t="s">
@@ -5197,93 +5225,93 @@
       <c r="BY36" s="82"/>
       <c r="BZ36" s="82"/>
     </row>
-    <row r="37" spans="1:78" s="105" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="156"/>
-      <c r="B37" s="157"/>
-      <c r="C37" s="158" t="s">
-        <v>121</v>
-      </c>
-      <c r="D37" s="159"/>
-      <c r="E37" s="159"/>
-      <c r="F37" s="159"/>
-      <c r="G37" s="159"/>
-      <c r="H37" s="159"/>
-      <c r="I37" s="160"/>
-      <c r="J37" s="161"/>
-      <c r="K37" s="162"/>
-      <c r="L37" s="162"/>
-      <c r="M37" s="160"/>
-      <c r="N37" s="160"/>
-      <c r="O37" s="160"/>
-      <c r="P37" s="160"/>
-      <c r="Q37" s="160"/>
-      <c r="R37" s="160"/>
-      <c r="S37" s="160"/>
-      <c r="T37" s="160"/>
-      <c r="U37" s="160"/>
-      <c r="V37" s="160"/>
-      <c r="W37" s="160"/>
-      <c r="X37" s="160"/>
-      <c r="Y37" s="160"/>
-      <c r="Z37" s="160"/>
-      <c r="AA37" s="160"/>
-      <c r="AB37" s="160"/>
-      <c r="AC37" s="160"/>
-      <c r="AD37" s="160"/>
-      <c r="AE37" s="160"/>
-      <c r="AF37" s="160"/>
-      <c r="AG37" s="160"/>
-      <c r="AH37" s="160"/>
-      <c r="AI37" s="160"/>
-      <c r="AJ37" s="163"/>
-      <c r="AK37" s="160"/>
-      <c r="AL37" s="160"/>
-      <c r="AM37" s="160"/>
-      <c r="AN37" s="160"/>
-      <c r="AO37" s="160"/>
-      <c r="AP37" s="160"/>
-      <c r="AQ37" s="160"/>
-      <c r="AR37" s="160"/>
-      <c r="AS37" s="160"/>
-      <c r="AT37" s="160"/>
-      <c r="AU37" s="160"/>
-      <c r="AV37" s="160"/>
-      <c r="AW37" s="160"/>
-      <c r="AX37" s="160"/>
-      <c r="AY37" s="160"/>
-      <c r="AZ37" s="160"/>
-      <c r="BA37" s="160"/>
-      <c r="BB37" s="160"/>
-      <c r="BC37" s="160"/>
-      <c r="BD37" s="160"/>
-      <c r="BE37" s="160"/>
-      <c r="BF37" s="160"/>
-      <c r="BG37" s="160"/>
-      <c r="BH37" s="160"/>
-      <c r="BI37" s="160"/>
-      <c r="BJ37" s="160"/>
-      <c r="BK37" s="160"/>
-      <c r="BL37" s="160"/>
-      <c r="BM37" s="160"/>
-      <c r="BN37" s="160"/>
-      <c r="BO37" s="160"/>
-      <c r="BP37" s="160"/>
-      <c r="BQ37" s="160"/>
-      <c r="BR37" s="160"/>
-      <c r="BS37" s="160"/>
-      <c r="BT37" s="160"/>
-      <c r="BU37" s="160"/>
-      <c r="BV37" s="160"/>
-      <c r="BW37" s="160"/>
-      <c r="BX37" s="160"/>
-      <c r="BY37" s="160"/>
-      <c r="BZ37" s="160"/>
+    <row r="37" spans="1:78" s="105" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="134"/>
+      <c r="B37" s="135"/>
+      <c r="C37" s="136" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" s="137"/>
+      <c r="E37" s="137"/>
+      <c r="F37" s="137"/>
+      <c r="G37" s="137"/>
+      <c r="H37" s="137"/>
+      <c r="I37" s="138"/>
+      <c r="J37" s="139"/>
+      <c r="K37" s="140"/>
+      <c r="L37" s="140"/>
+      <c r="M37" s="138"/>
+      <c r="N37" s="138"/>
+      <c r="O37" s="138"/>
+      <c r="P37" s="138"/>
+      <c r="Q37" s="138"/>
+      <c r="R37" s="138"/>
+      <c r="S37" s="138"/>
+      <c r="T37" s="138"/>
+      <c r="U37" s="138"/>
+      <c r="V37" s="138"/>
+      <c r="W37" s="138"/>
+      <c r="X37" s="138"/>
+      <c r="Y37" s="138"/>
+      <c r="Z37" s="138"/>
+      <c r="AA37" s="138"/>
+      <c r="AB37" s="138"/>
+      <c r="AC37" s="138"/>
+      <c r="AD37" s="138"/>
+      <c r="AE37" s="138"/>
+      <c r="AF37" s="138"/>
+      <c r="AG37" s="138"/>
+      <c r="AH37" s="138"/>
+      <c r="AI37" s="138"/>
+      <c r="AJ37" s="141"/>
+      <c r="AK37" s="138"/>
+      <c r="AL37" s="138"/>
+      <c r="AM37" s="138"/>
+      <c r="AN37" s="138"/>
+      <c r="AO37" s="138"/>
+      <c r="AP37" s="138"/>
+      <c r="AQ37" s="138"/>
+      <c r="AR37" s="138"/>
+      <c r="AS37" s="138"/>
+      <c r="AT37" s="138"/>
+      <c r="AU37" s="138"/>
+      <c r="AV37" s="138"/>
+      <c r="AW37" s="138"/>
+      <c r="AX37" s="138"/>
+      <c r="AY37" s="138"/>
+      <c r="AZ37" s="138"/>
+      <c r="BA37" s="138"/>
+      <c r="BB37" s="138"/>
+      <c r="BC37" s="138"/>
+      <c r="BD37" s="138"/>
+      <c r="BE37" s="138"/>
+      <c r="BF37" s="138"/>
+      <c r="BG37" s="138"/>
+      <c r="BH37" s="138"/>
+      <c r="BI37" s="138"/>
+      <c r="BJ37" s="138"/>
+      <c r="BK37" s="138"/>
+      <c r="BL37" s="138"/>
+      <c r="BM37" s="138"/>
+      <c r="BN37" s="138"/>
+      <c r="BO37" s="138"/>
+      <c r="BP37" s="138"/>
+      <c r="BQ37" s="138"/>
+      <c r="BR37" s="138"/>
+      <c r="BS37" s="138"/>
+      <c r="BT37" s="138"/>
+      <c r="BU37" s="138"/>
+      <c r="BV37" s="138"/>
+      <c r="BW37" s="138"/>
+      <c r="BX37" s="138"/>
+      <c r="BY37" s="138"/>
+      <c r="BZ37" s="138"/>
     </row>
-    <row r="38" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="21"/>
       <c r="B38" s="85"/>
       <c r="C38" s="120" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D38" s="87"/>
       <c r="E38" s="87"/>
@@ -5361,11 +5389,11 @@
       <c r="BY38" s="88"/>
       <c r="BZ38" s="88"/>
     </row>
-    <row r="39" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="21"/>
       <c r="B39" s="85"/>
       <c r="C39" s="120" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D39" s="87"/>
       <c r="E39" s="87"/>
@@ -5399,9 +5427,9 @@
       <c r="AG39" s="88"/>
       <c r="AH39" s="88"/>
       <c r="AI39" s="88"/>
-      <c r="AJ39" s="170"/>
-      <c r="AK39" s="170"/>
-      <c r="AL39" s="170"/>
+      <c r="AJ39" s="148"/>
+      <c r="AK39" s="148"/>
+      <c r="AL39" s="148"/>
       <c r="AM39" s="88"/>
       <c r="AN39" s="88"/>
       <c r="AO39" s="121"/>
@@ -5409,7 +5437,7 @@
       <c r="AQ39" s="121"/>
       <c r="AR39" s="122"/>
       <c r="AS39" s="122"/>
-      <c r="AT39" s="169"/>
+      <c r="AT39" s="147"/>
       <c r="AU39" s="88"/>
       <c r="AV39" s="88"/>
       <c r="AW39" s="88"/>
@@ -5443,11 +5471,11 @@
       <c r="BY39" s="88"/>
       <c r="BZ39" s="88"/>
     </row>
-    <row r="40" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="21"/>
       <c r="B40" s="85"/>
       <c r="C40" s="120" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D40" s="87"/>
       <c r="E40" s="87"/>
@@ -5481,9 +5509,9 @@
       <c r="AG40" s="88"/>
       <c r="AH40" s="88"/>
       <c r="AI40" s="88"/>
-      <c r="AJ40" s="170"/>
-      <c r="AK40" s="170"/>
-      <c r="AL40" s="170"/>
+      <c r="AJ40" s="148"/>
+      <c r="AK40" s="148"/>
+      <c r="AL40" s="148"/>
       <c r="AM40" s="88"/>
       <c r="AN40" s="88"/>
       <c r="AO40" s="121"/>
@@ -5525,11 +5553,11 @@
       <c r="BY40" s="88"/>
       <c r="BZ40" s="88"/>
     </row>
-    <row r="41" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="21"/>
       <c r="B41" s="85"/>
       <c r="C41" s="120" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D41" s="87"/>
       <c r="E41" s="87"/>
@@ -5563,9 +5591,9 @@
       <c r="AG41" s="88"/>
       <c r="AH41" s="88"/>
       <c r="AI41" s="88"/>
-      <c r="AJ41" s="170"/>
-      <c r="AK41" s="170"/>
-      <c r="AL41" s="170"/>
+      <c r="AJ41" s="148"/>
+      <c r="AK41" s="148"/>
+      <c r="AL41" s="148"/>
       <c r="AM41" s="88"/>
       <c r="AN41" s="88"/>
       <c r="AO41" s="121"/>
@@ -5607,11 +5635,11 @@
       <c r="BY41" s="88"/>
       <c r="BZ41" s="88"/>
     </row>
-    <row r="42" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="21"/>
       <c r="B42" s="85"/>
       <c r="C42" s="120" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D42" s="87"/>
       <c r="E42" s="87"/>
@@ -5645,9 +5673,9 @@
       <c r="AG42" s="88"/>
       <c r="AH42" s="88"/>
       <c r="AI42" s="88"/>
-      <c r="AJ42" s="170"/>
-      <c r="AK42" s="170"/>
-      <c r="AL42" s="170"/>
+      <c r="AJ42" s="148"/>
+      <c r="AK42" s="148"/>
+      <c r="AL42" s="148"/>
       <c r="AM42" s="88"/>
       <c r="AN42" s="88"/>
       <c r="AO42" s="88"/>
@@ -5689,7 +5717,7 @@
       <c r="BY42" s="88"/>
       <c r="BZ42" s="88"/>
     </row>
-    <row r="43" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="21"/>
       <c r="B43" s="85"/>
       <c r="C43" s="120"/>
@@ -5725,9 +5753,9 @@
       <c r="AG43" s="88"/>
       <c r="AH43" s="88"/>
       <c r="AI43" s="88"/>
-      <c r="AJ43" s="170"/>
-      <c r="AK43" s="170"/>
-      <c r="AL43" s="170"/>
+      <c r="AJ43" s="148"/>
+      <c r="AK43" s="148"/>
+      <c r="AL43" s="148"/>
       <c r="AM43" s="88"/>
       <c r="AN43" s="88"/>
       <c r="AO43" s="88"/>
@@ -5769,93 +5797,93 @@
       <c r="BY43" s="88"/>
       <c r="BZ43" s="88"/>
     </row>
-    <row r="44" spans="1:78" s="105" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="156"/>
-      <c r="B44" s="164"/>
-      <c r="C44" s="165" t="s">
+    <row r="44" spans="1:78" s="105" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="134"/>
+      <c r="B44" s="142"/>
+      <c r="C44" s="143" t="s">
         <v>31</v>
       </c>
-      <c r="D44" s="166"/>
-      <c r="E44" s="166"/>
-      <c r="F44" s="166"/>
-      <c r="G44" s="166"/>
-      <c r="H44" s="166"/>
-      <c r="I44" s="163"/>
-      <c r="J44" s="167"/>
-      <c r="K44" s="168"/>
-      <c r="L44" s="168"/>
-      <c r="M44" s="163"/>
-      <c r="N44" s="163"/>
-      <c r="O44" s="163"/>
-      <c r="P44" s="163"/>
-      <c r="Q44" s="163"/>
-      <c r="R44" s="163"/>
-      <c r="S44" s="163"/>
-      <c r="T44" s="163"/>
-      <c r="U44" s="163"/>
-      <c r="V44" s="163"/>
-      <c r="W44" s="163"/>
-      <c r="X44" s="163"/>
-      <c r="Y44" s="163"/>
-      <c r="Z44" s="163"/>
-      <c r="AA44" s="163"/>
-      <c r="AB44" s="163"/>
-      <c r="AC44" s="163"/>
-      <c r="AD44" s="163"/>
-      <c r="AE44" s="163"/>
-      <c r="AF44" s="163"/>
-      <c r="AG44" s="163"/>
-      <c r="AH44" s="163"/>
-      <c r="AI44" s="163"/>
-      <c r="AJ44" s="163"/>
-      <c r="AK44" s="163"/>
-      <c r="AL44" s="163"/>
-      <c r="AM44" s="163"/>
-      <c r="AN44" s="163"/>
-      <c r="AO44" s="163"/>
-      <c r="AP44" s="163"/>
-      <c r="AQ44" s="163"/>
-      <c r="AR44" s="163"/>
-      <c r="AS44" s="163"/>
-      <c r="AT44" s="163"/>
-      <c r="AU44" s="163"/>
-      <c r="AV44" s="163"/>
-      <c r="AW44" s="163"/>
-      <c r="AX44" s="163"/>
-      <c r="AY44" s="163"/>
-      <c r="AZ44" s="163"/>
-      <c r="BA44" s="163"/>
-      <c r="BB44" s="163"/>
-      <c r="BC44" s="163"/>
-      <c r="BD44" s="163"/>
-      <c r="BE44" s="163"/>
-      <c r="BF44" s="163"/>
-      <c r="BG44" s="163"/>
-      <c r="BH44" s="163"/>
-      <c r="BI44" s="163"/>
-      <c r="BJ44" s="163"/>
-      <c r="BK44" s="163"/>
-      <c r="BL44" s="163"/>
-      <c r="BM44" s="163"/>
-      <c r="BN44" s="163"/>
-      <c r="BO44" s="163"/>
-      <c r="BP44" s="163"/>
-      <c r="BQ44" s="163"/>
-      <c r="BR44" s="163"/>
-      <c r="BS44" s="163"/>
-      <c r="BT44" s="163"/>
-      <c r="BU44" s="163"/>
-      <c r="BV44" s="163"/>
-      <c r="BW44" s="163"/>
-      <c r="BX44" s="163"/>
-      <c r="BY44" s="163"/>
-      <c r="BZ44" s="163"/>
+      <c r="D44" s="144"/>
+      <c r="E44" s="144"/>
+      <c r="F44" s="144"/>
+      <c r="G44" s="144"/>
+      <c r="H44" s="144"/>
+      <c r="I44" s="141"/>
+      <c r="J44" s="145"/>
+      <c r="K44" s="146"/>
+      <c r="L44" s="146"/>
+      <c r="M44" s="141"/>
+      <c r="N44" s="141"/>
+      <c r="O44" s="141"/>
+      <c r="P44" s="141"/>
+      <c r="Q44" s="141"/>
+      <c r="R44" s="141"/>
+      <c r="S44" s="141"/>
+      <c r="T44" s="141"/>
+      <c r="U44" s="141"/>
+      <c r="V44" s="141"/>
+      <c r="W44" s="141"/>
+      <c r="X44" s="141"/>
+      <c r="Y44" s="141"/>
+      <c r="Z44" s="141"/>
+      <c r="AA44" s="141"/>
+      <c r="AB44" s="141"/>
+      <c r="AC44" s="141"/>
+      <c r="AD44" s="141"/>
+      <c r="AE44" s="141"/>
+      <c r="AF44" s="141"/>
+      <c r="AG44" s="141"/>
+      <c r="AH44" s="141"/>
+      <c r="AI44" s="141"/>
+      <c r="AJ44" s="141"/>
+      <c r="AK44" s="141"/>
+      <c r="AL44" s="141"/>
+      <c r="AM44" s="141"/>
+      <c r="AN44" s="141"/>
+      <c r="AO44" s="141"/>
+      <c r="AP44" s="141"/>
+      <c r="AQ44" s="141"/>
+      <c r="AR44" s="141"/>
+      <c r="AS44" s="141"/>
+      <c r="AT44" s="141"/>
+      <c r="AU44" s="141"/>
+      <c r="AV44" s="141"/>
+      <c r="AW44" s="141"/>
+      <c r="AX44" s="141"/>
+      <c r="AY44" s="141"/>
+      <c r="AZ44" s="141"/>
+      <c r="BA44" s="141"/>
+      <c r="BB44" s="141"/>
+      <c r="BC44" s="141"/>
+      <c r="BD44" s="141"/>
+      <c r="BE44" s="141"/>
+      <c r="BF44" s="141"/>
+      <c r="BG44" s="141"/>
+      <c r="BH44" s="141"/>
+      <c r="BI44" s="141"/>
+      <c r="BJ44" s="141"/>
+      <c r="BK44" s="141"/>
+      <c r="BL44" s="141"/>
+      <c r="BM44" s="141"/>
+      <c r="BN44" s="141"/>
+      <c r="BO44" s="141"/>
+      <c r="BP44" s="141"/>
+      <c r="BQ44" s="141"/>
+      <c r="BR44" s="141"/>
+      <c r="BS44" s="141"/>
+      <c r="BT44" s="141"/>
+      <c r="BU44" s="141"/>
+      <c r="BV44" s="141"/>
+      <c r="BW44" s="141"/>
+      <c r="BX44" s="141"/>
+      <c r="BY44" s="141"/>
+      <c r="BZ44" s="141"/>
     </row>
-    <row r="45" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="21"/>
       <c r="B45" s="85"/>
       <c r="C45" s="120" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D45" s="87"/>
       <c r="E45" s="87"/>
@@ -5933,11 +5961,11 @@
       <c r="BY45" s="88"/>
       <c r="BZ45" s="88"/>
     </row>
-    <row r="46" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="21"/>
       <c r="B46" s="85"/>
       <c r="C46" s="120" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D46" s="87"/>
       <c r="E46" s="87"/>
@@ -6015,11 +6043,11 @@
       <c r="BY46" s="88"/>
       <c r="BZ46" s="88"/>
     </row>
-    <row r="47" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="21"/>
       <c r="B47" s="85"/>
       <c r="C47" s="120" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D47" s="87"/>
       <c r="E47" s="87"/>
@@ -6097,11 +6125,11 @@
       <c r="BY47" s="88"/>
       <c r="BZ47" s="88"/>
     </row>
-    <row r="48" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="21"/>
       <c r="B48" s="85"/>
       <c r="C48" s="120" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D48" s="87"/>
       <c r="E48" s="87"/>
@@ -6139,7 +6167,7 @@
       <c r="AK48" s="88"/>
       <c r="AL48" s="88"/>
       <c r="AM48" s="88"/>
-      <c r="AN48" s="170"/>
+      <c r="AN48" s="148"/>
       <c r="AO48" s="121"/>
       <c r="AP48" s="121"/>
       <c r="AQ48" s="121"/>
@@ -6179,7 +6207,7 @@
       <c r="BY48" s="88"/>
       <c r="BZ48" s="88"/>
     </row>
-    <row r="49" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:78" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="21"/>
       <c r="B49" s="85"/>
       <c r="C49" s="86"/>
@@ -6259,7 +6287,7 @@
       <c r="BY49" s="88"/>
       <c r="BZ49" s="88"/>
     </row>
-    <row r="50" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A50" s="72"/>
       <c r="B50" s="73"/>
       <c r="C50" s="76" t="s">
@@ -6341,11 +6369,11 @@
       <c r="BY50" s="67"/>
       <c r="BZ50" s="67"/>
     </row>
-    <row r="51" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A51" s="32"/>
       <c r="B51" s="53"/>
       <c r="C51" s="56" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D51" s="54"/>
       <c r="E51" s="35"/>
@@ -6423,11 +6451,11 @@
       <c r="BY51" s="38"/>
       <c r="BZ51" s="38"/>
     </row>
-    <row r="52" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A52" s="32"/>
       <c r="B52" s="53"/>
       <c r="C52" s="56" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D52" s="54"/>
       <c r="E52" s="35"/>
@@ -6505,11 +6533,11 @@
       <c r="BY52" s="38"/>
       <c r="BZ52" s="38"/>
     </row>
-    <row r="53" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A53" s="32"/>
       <c r="B53" s="53"/>
       <c r="C53" s="56" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D53" s="54"/>
       <c r="E53" s="35"/>
@@ -6587,7 +6615,7 @@
       <c r="BY53" s="38"/>
       <c r="BZ53" s="38"/>
     </row>
-    <row r="54" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A54" s="32"/>
       <c r="B54" s="53"/>
       <c r="C54" s="56" t="s">
@@ -6669,7 +6697,7 @@
       <c r="BY54" s="38"/>
       <c r="BZ54" s="38"/>
     </row>
-    <row r="55" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A55" s="32"/>
       <c r="B55" s="53"/>
       <c r="C55" s="56" t="s">
@@ -6751,7 +6779,7 @@
       <c r="BY55" s="38"/>
       <c r="BZ55" s="38"/>
     </row>
-    <row r="56" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A56" s="32"/>
       <c r="B56" s="53"/>
       <c r="C56" s="56" t="s">
@@ -6833,11 +6861,11 @@
       <c r="BY56" s="38"/>
       <c r="BZ56" s="38"/>
     </row>
-    <row r="57" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A57" s="32"/>
       <c r="B57" s="53"/>
       <c r="C57" s="56" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D57" s="54"/>
       <c r="E57" s="35"/>
@@ -6915,11 +6943,11 @@
       <c r="BY57" s="38"/>
       <c r="BZ57" s="38"/>
     </row>
-    <row r="58" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A58" s="32"/>
       <c r="B58" s="53"/>
       <c r="C58" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D58" s="54"/>
       <c r="E58" s="35"/>
@@ -6997,7 +7025,7 @@
       <c r="BY58" s="38"/>
       <c r="BZ58" s="38"/>
     </row>
-    <row r="59" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A59" s="32"/>
       <c r="B59" s="53"/>
       <c r="C59" s="56" t="s">
@@ -7079,7 +7107,7 @@
       <c r="BY59" s="38"/>
       <c r="BZ59" s="38"/>
     </row>
-    <row r="60" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A60" s="32"/>
       <c r="B60" s="53"/>
       <c r="C60" s="56" t="s">
@@ -7161,7 +7189,7 @@
       <c r="BY60" s="38"/>
       <c r="BZ60" s="38"/>
     </row>
-    <row r="61" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A61" s="32"/>
       <c r="B61" s="53"/>
       <c r="C61" s="56" t="s">
@@ -7243,7 +7271,7 @@
       <c r="BY61" s="38"/>
       <c r="BZ61" s="38"/>
     </row>
-    <row r="62" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A62" s="32"/>
       <c r="B62" s="53"/>
       <c r="C62" s="56" t="s">
@@ -7325,7 +7353,7 @@
       <c r="BY62" s="38"/>
       <c r="BZ62" s="38"/>
     </row>
-    <row r="63" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A63" s="32"/>
       <c r="B63" s="53"/>
       <c r="C63" s="56"/>
@@ -7405,7 +7433,7 @@
       <c r="BY63" s="38"/>
       <c r="BZ63" s="38"/>
     </row>
-    <row r="64" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A64" s="32"/>
       <c r="B64" s="59"/>
       <c r="C64" s="60" t="s">
@@ -7487,7 +7515,7 @@
       <c r="BY64" s="67"/>
       <c r="BZ64" s="67"/>
     </row>
-    <row r="65" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A65" s="32"/>
       <c r="B65" s="53"/>
       <c r="C65" s="56" t="s">
@@ -7569,7 +7597,7 @@
       <c r="BY65" s="38"/>
       <c r="BZ65" s="38"/>
     </row>
-    <row r="66" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A66" s="32"/>
       <c r="B66" s="53"/>
       <c r="C66" s="56" t="s">
@@ -7651,7 +7679,7 @@
       <c r="BY66" s="38"/>
       <c r="BZ66" s="38"/>
     </row>
-    <row r="67" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A67" s="32"/>
       <c r="B67" s="53"/>
       <c r="C67" s="56" t="s">
@@ -7733,7 +7761,7 @@
       <c r="BY67" s="38"/>
       <c r="BZ67" s="38"/>
     </row>
-    <row r="68" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A68" s="32"/>
       <c r="B68" s="53"/>
       <c r="C68" s="56" t="s">
@@ -7815,7 +7843,7 @@
       <c r="BY68" s="38"/>
       <c r="BZ68" s="38"/>
     </row>
-    <row r="69" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A69" s="32"/>
       <c r="B69" s="53"/>
       <c r="C69" s="56" t="s">
@@ -7897,11 +7925,11 @@
       <c r="BY69" s="38"/>
       <c r="BZ69" s="38"/>
     </row>
-    <row r="70" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A70" s="32"/>
       <c r="B70" s="53"/>
       <c r="C70" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D70" s="54"/>
       <c r="E70" s="35"/>
@@ -7979,7 +8007,7 @@
       <c r="BY70" s="38"/>
       <c r="BZ70" s="38"/>
     </row>
-    <row r="71" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A71" s="32"/>
       <c r="B71" s="53"/>
       <c r="C71" s="56"/>
@@ -8059,7 +8087,7 @@
       <c r="BY71" s="38"/>
       <c r="BZ71" s="38"/>
     </row>
-    <row r="72" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A72" s="32"/>
       <c r="B72" s="53"/>
       <c r="C72" s="56"/>
@@ -8139,7 +8167,7 @@
       <c r="BY72" s="38"/>
       <c r="BZ72" s="38"/>
     </row>
-    <row r="73" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A73" s="32"/>
       <c r="B73" s="53"/>
       <c r="C73" s="56"/>
@@ -8219,7 +8247,7 @@
       <c r="BY73" s="38"/>
       <c r="BZ73" s="38"/>
     </row>
-    <row r="74" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A74" s="72"/>
       <c r="B74" s="59"/>
       <c r="C74" s="60" t="s">
@@ -8301,7 +8329,7 @@
       <c r="BY74" s="67"/>
       <c r="BZ74" s="67"/>
     </row>
-    <row r="75" spans="1:78" s="105" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:78" s="105" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A75" s="91"/>
       <c r="B75" s="92"/>
       <c r="C75" s="93" t="s">
@@ -8383,11 +8411,11 @@
       <c r="BY75" s="100"/>
       <c r="BZ75" s="100"/>
     </row>
-    <row r="76" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A76" s="32"/>
       <c r="B76" s="53"/>
       <c r="C76" s="56" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="D76" s="54"/>
       <c r="E76" s="35"/>
@@ -8465,11 +8493,11 @@
       <c r="BY76" s="38"/>
       <c r="BZ76" s="38"/>
     </row>
-    <row r="77" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A77" s="32"/>
       <c r="B77" s="53"/>
       <c r="C77" s="56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D77" s="54"/>
       <c r="E77" s="35"/>
@@ -8501,11 +8529,11 @@
       <c r="AE77" s="38"/>
       <c r="AF77" s="38"/>
       <c r="AG77" s="38"/>
-      <c r="AH77" s="39"/>
-      <c r="AI77" s="39"/>
-      <c r="AJ77" s="38"/>
-      <c r="AK77" s="39"/>
-      <c r="AL77" s="39"/>
+      <c r="AH77" s="171"/>
+      <c r="AI77" s="171"/>
+      <c r="AJ77" s="171"/>
+      <c r="AK77" s="171"/>
+      <c r="AL77" s="171"/>
       <c r="AM77" s="38"/>
       <c r="AN77" s="38"/>
       <c r="AO77" s="38"/>
@@ -8547,11 +8575,11 @@
       <c r="BY77" s="38"/>
       <c r="BZ77" s="38"/>
     </row>
-    <row r="78" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A78" s="32"/>
       <c r="B78" s="53"/>
       <c r="C78" s="56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D78" s="54"/>
       <c r="E78" s="35"/>
@@ -8583,11 +8611,11 @@
       <c r="AE78" s="38"/>
       <c r="AF78" s="38"/>
       <c r="AG78" s="38"/>
-      <c r="AH78" s="39"/>
-      <c r="AI78" s="39"/>
-      <c r="AJ78" s="38"/>
-      <c r="AK78" s="39"/>
-      <c r="AL78" s="39"/>
+      <c r="AH78" s="171"/>
+      <c r="AI78" s="171"/>
+      <c r="AJ78" s="171"/>
+      <c r="AK78" s="171"/>
+      <c r="AL78" s="171"/>
       <c r="AM78" s="38"/>
       <c r="AN78" s="38"/>
       <c r="AO78" s="38"/>
@@ -8629,11 +8657,11 @@
       <c r="BY78" s="38"/>
       <c r="BZ78" s="38"/>
     </row>
-    <row r="79" spans="1:78" ht="16.8" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:78" ht="16.75" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A79" s="32"/>
       <c r="B79" s="53"/>
       <c r="C79" s="56" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="D79" s="54"/>
       <c r="E79" s="35"/>
@@ -8665,9 +8693,9 @@
       <c r="AE79" s="38"/>
       <c r="AF79" s="38"/>
       <c r="AG79" s="38"/>
-      <c r="AH79" s="39"/>
-      <c r="AI79" s="39"/>
-      <c r="AJ79" s="38"/>
+      <c r="AH79" s="171"/>
+      <c r="AI79" s="171"/>
+      <c r="AJ79" s="171"/>
       <c r="AK79" s="123"/>
       <c r="AL79" s="123"/>
       <c r="AM79" s="58"/>
@@ -8711,11 +8739,11 @@
       <c r="BY79" s="38"/>
       <c r="BZ79" s="38"/>
     </row>
-    <row r="80" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A80" s="32"/>
       <c r="B80" s="53"/>
       <c r="C80" s="56" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D80" s="54"/>
       <c r="E80" s="35"/>
@@ -8747,9 +8775,9 @@
       <c r="AE80" s="38"/>
       <c r="AF80" s="38"/>
       <c r="AG80" s="38"/>
-      <c r="AH80" s="39"/>
-      <c r="AI80" s="39"/>
-      <c r="AJ80" s="38"/>
+      <c r="AH80" s="171"/>
+      <c r="AI80" s="171"/>
+      <c r="AJ80" s="171"/>
       <c r="AK80" s="123"/>
       <c r="AL80" s="123"/>
       <c r="AM80" s="58"/>
@@ -8793,11 +8821,11 @@
       <c r="BY80" s="38"/>
       <c r="BZ80" s="38"/>
     </row>
-    <row r="81" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A81" s="32"/>
       <c r="B81" s="53"/>
       <c r="C81" s="56" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D81" s="54"/>
       <c r="E81" s="35"/>
@@ -8829,9 +8857,9 @@
       <c r="AE81" s="38"/>
       <c r="AF81" s="38"/>
       <c r="AG81" s="38"/>
-      <c r="AH81" s="39"/>
-      <c r="AI81" s="39"/>
-      <c r="AJ81" s="38"/>
+      <c r="AH81" s="171"/>
+      <c r="AI81" s="171"/>
+      <c r="AJ81" s="171"/>
       <c r="AK81" s="123"/>
       <c r="AL81" s="123"/>
       <c r="AM81" s="58"/>
@@ -8875,10 +8903,12 @@
       <c r="BY81" s="38"/>
       <c r="BZ81" s="38"/>
     </row>
-    <row r="82" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A82" s="32"/>
       <c r="B82" s="53"/>
-      <c r="C82" s="56"/>
+      <c r="C82" s="56" t="s">
+        <v>130</v>
+      </c>
       <c r="D82" s="54"/>
       <c r="E82" s="35"/>
       <c r="F82" s="35"/>
@@ -8904,22 +8934,22 @@
       <c r="Z82" s="38"/>
       <c r="AA82" s="38"/>
       <c r="AB82" s="38"/>
-      <c r="AC82" s="39"/>
-      <c r="AD82" s="39"/>
-      <c r="AE82" s="39"/>
-      <c r="AF82" s="39"/>
-      <c r="AG82" s="39"/>
-      <c r="AH82" s="38"/>
-      <c r="AI82" s="38"/>
-      <c r="AJ82" s="38"/>
-      <c r="AK82" s="38"/>
-      <c r="AL82" s="38"/>
-      <c r="AM82" s="38"/>
+      <c r="AC82" s="38"/>
+      <c r="AD82" s="38"/>
+      <c r="AE82" s="38"/>
+      <c r="AF82" s="38"/>
+      <c r="AG82" s="38"/>
+      <c r="AH82" s="171"/>
+      <c r="AI82" s="171"/>
+      <c r="AJ82" s="171"/>
+      <c r="AK82" s="171"/>
+      <c r="AL82" s="171"/>
+      <c r="AM82" s="171"/>
       <c r="AN82" s="38"/>
-      <c r="AO82" s="38"/>
-      <c r="AP82" s="38"/>
-      <c r="AQ82" s="38"/>
-      <c r="AR82" s="40"/>
+      <c r="AO82" s="124"/>
+      <c r="AP82" s="124"/>
+      <c r="AQ82" s="124"/>
+      <c r="AR82" s="172"/>
       <c r="AS82" s="40"/>
       <c r="AT82" s="40"/>
       <c r="AU82" s="40"/>
@@ -8955,94 +8985,92 @@
       <c r="BY82" s="38"/>
       <c r="BZ82" s="38"/>
     </row>
-    <row r="83" spans="1:78" s="105" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="91"/>
-      <c r="B83" s="92"/>
-      <c r="C83" s="93" t="s">
-        <v>90</v>
-      </c>
-      <c r="D83" s="94"/>
-      <c r="E83" s="95"/>
-      <c r="F83" s="95"/>
-      <c r="G83" s="96"/>
-      <c r="H83" s="97"/>
-      <c r="I83" s="98"/>
-      <c r="J83" s="99"/>
-      <c r="K83" s="100"/>
-      <c r="L83" s="100"/>
-      <c r="M83" s="100"/>
-      <c r="N83" s="101"/>
-      <c r="O83" s="101"/>
-      <c r="P83" s="101"/>
-      <c r="Q83" s="101"/>
-      <c r="R83" s="101"/>
-      <c r="S83" s="100"/>
-      <c r="T83" s="100"/>
-      <c r="U83" s="100"/>
-      <c r="V83" s="100"/>
-      <c r="W83" s="100"/>
-      <c r="X83" s="100"/>
-      <c r="Y83" s="100"/>
-      <c r="Z83" s="100"/>
-      <c r="AA83" s="100"/>
-      <c r="AB83" s="100"/>
-      <c r="AC83" s="102"/>
-      <c r="AD83" s="102"/>
-      <c r="AE83" s="102"/>
-      <c r="AF83" s="102"/>
-      <c r="AG83" s="102"/>
-      <c r="AH83" s="100"/>
-      <c r="AI83" s="100"/>
-      <c r="AJ83" s="100"/>
-      <c r="AK83" s="100"/>
-      <c r="AL83" s="100"/>
-      <c r="AM83" s="100"/>
-      <c r="AN83" s="100"/>
-      <c r="AO83" s="100"/>
-      <c r="AP83" s="100"/>
-      <c r="AQ83" s="100"/>
-      <c r="AR83" s="103"/>
-      <c r="AS83" s="103"/>
-      <c r="AT83" s="103"/>
-      <c r="AU83" s="103"/>
-      <c r="AV83" s="103"/>
-      <c r="AW83" s="100"/>
-      <c r="AX83" s="100"/>
-      <c r="AY83" s="100"/>
-      <c r="AZ83" s="100"/>
-      <c r="BA83" s="100"/>
-      <c r="BB83" s="100"/>
-      <c r="BC83" s="100"/>
-      <c r="BD83" s="100"/>
-      <c r="BE83" s="100"/>
-      <c r="BF83" s="100"/>
-      <c r="BG83" s="104"/>
-      <c r="BH83" s="104"/>
-      <c r="BI83" s="104"/>
-      <c r="BJ83" s="104"/>
-      <c r="BK83" s="104"/>
-      <c r="BL83" s="100"/>
-      <c r="BM83" s="100"/>
-      <c r="BN83" s="100"/>
-      <c r="BO83" s="100"/>
-      <c r="BP83" s="100"/>
-      <c r="BQ83" s="100"/>
-      <c r="BR83" s="100"/>
-      <c r="BS83" s="100"/>
-      <c r="BT83" s="100"/>
-      <c r="BU83" s="100"/>
-      <c r="BV83" s="100"/>
-      <c r="BW83" s="100"/>
-      <c r="BX83" s="100"/>
-      <c r="BY83" s="100"/>
-      <c r="BZ83" s="100"/>
+    <row r="83" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="32"/>
+      <c r="B83" s="53"/>
+      <c r="C83" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="D83" s="54"/>
+      <c r="E83" s="35"/>
+      <c r="F83" s="35"/>
+      <c r="G83" s="36"/>
+      <c r="H83" s="37"/>
+      <c r="I83" s="42"/>
+      <c r="J83" s="43"/>
+      <c r="K83" s="38"/>
+      <c r="L83" s="38"/>
+      <c r="M83" s="38"/>
+      <c r="N83" s="44"/>
+      <c r="O83" s="44"/>
+      <c r="P83" s="44"/>
+      <c r="Q83" s="44"/>
+      <c r="R83" s="44"/>
+      <c r="S83" s="38"/>
+      <c r="T83" s="38"/>
+      <c r="U83" s="38"/>
+      <c r="V83" s="38"/>
+      <c r="W83" s="38"/>
+      <c r="X83" s="38"/>
+      <c r="Y83" s="38"/>
+      <c r="Z83" s="38"/>
+      <c r="AA83" s="38"/>
+      <c r="AB83" s="38"/>
+      <c r="AC83" s="38"/>
+      <c r="AD83" s="38"/>
+      <c r="AE83" s="38"/>
+      <c r="AF83" s="38"/>
+      <c r="AG83" s="38"/>
+      <c r="AH83" s="171"/>
+      <c r="AI83" s="171"/>
+      <c r="AJ83" s="171"/>
+      <c r="AK83" s="171"/>
+      <c r="AL83" s="171"/>
+      <c r="AM83" s="171"/>
+      <c r="AN83" s="38"/>
+      <c r="AO83" s="124"/>
+      <c r="AP83" s="124"/>
+      <c r="AQ83" s="124"/>
+      <c r="AR83" s="172"/>
+      <c r="AS83" s="40"/>
+      <c r="AT83" s="40"/>
+      <c r="AU83" s="40"/>
+      <c r="AV83" s="40"/>
+      <c r="AW83" s="38"/>
+      <c r="AX83" s="38"/>
+      <c r="AY83" s="38"/>
+      <c r="AZ83" s="38"/>
+      <c r="BA83" s="38"/>
+      <c r="BB83" s="38"/>
+      <c r="BC83" s="38"/>
+      <c r="BD83" s="38"/>
+      <c r="BE83" s="38"/>
+      <c r="BF83" s="38"/>
+      <c r="BG83" s="41"/>
+      <c r="BH83" s="41"/>
+      <c r="BI83" s="41"/>
+      <c r="BJ83" s="41"/>
+      <c r="BK83" s="41"/>
+      <c r="BL83" s="38"/>
+      <c r="BM83" s="38"/>
+      <c r="BN83" s="38"/>
+      <c r="BO83" s="38"/>
+      <c r="BP83" s="38"/>
+      <c r="BQ83" s="38"/>
+      <c r="BR83" s="38"/>
+      <c r="BS83" s="38"/>
+      <c r="BT83" s="38"/>
+      <c r="BU83" s="38"/>
+      <c r="BV83" s="38"/>
+      <c r="BW83" s="38"/>
+      <c r="BX83" s="38"/>
+      <c r="BY83" s="38"/>
+      <c r="BZ83" s="38"/>
     </row>
-    <row r="84" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A84" s="32"/>
       <c r="B84" s="53"/>
-      <c r="C84" s="56" t="s">
-        <v>97</v>
-      </c>
+      <c r="C84" s="56"/>
       <c r="D84" s="54"/>
       <c r="E84" s="35"/>
       <c r="F84" s="35"/>
@@ -9053,11 +9081,11 @@
       <c r="K84" s="38"/>
       <c r="L84" s="38"/>
       <c r="M84" s="38"/>
-      <c r="N84" s="38"/>
-      <c r="O84" s="38"/>
-      <c r="P84" s="38"/>
-      <c r="Q84" s="38"/>
-      <c r="R84" s="38"/>
+      <c r="N84" s="44"/>
+      <c r="O84" s="44"/>
+      <c r="P84" s="44"/>
+      <c r="Q84" s="44"/>
+      <c r="R84" s="44"/>
       <c r="S84" s="38"/>
       <c r="T84" s="38"/>
       <c r="U84" s="38"/>
@@ -9073,21 +9101,21 @@
       <c r="AE84" s="38"/>
       <c r="AF84" s="38"/>
       <c r="AG84" s="38"/>
-      <c r="AH84" s="38"/>
-      <c r="AI84" s="38"/>
-      <c r="AJ84" s="38"/>
-      <c r="AK84" s="38"/>
-      <c r="AL84" s="38"/>
-      <c r="AM84" s="38"/>
+      <c r="AH84" s="171"/>
+      <c r="AI84" s="171"/>
+      <c r="AJ84" s="171"/>
+      <c r="AK84" s="171"/>
+      <c r="AL84" s="171"/>
+      <c r="AM84" s="171"/>
       <c r="AN84" s="38"/>
       <c r="AO84" s="38"/>
       <c r="AP84" s="38"/>
       <c r="AQ84" s="38"/>
-      <c r="AR84" s="38"/>
-      <c r="AS84" s="38"/>
-      <c r="AT84" s="38"/>
-      <c r="AU84" s="38"/>
-      <c r="AV84" s="38"/>
+      <c r="AR84" s="40"/>
+      <c r="AS84" s="40"/>
+      <c r="AT84" s="40"/>
+      <c r="AU84" s="40"/>
+      <c r="AV84" s="40"/>
       <c r="AW84" s="38"/>
       <c r="AX84" s="38"/>
       <c r="AY84" s="38"/>
@@ -9098,11 +9126,11 @@
       <c r="BD84" s="38"/>
       <c r="BE84" s="38"/>
       <c r="BF84" s="38"/>
-      <c r="BG84" s="38"/>
-      <c r="BH84" s="38"/>
-      <c r="BI84" s="38"/>
-      <c r="BJ84" s="38"/>
-      <c r="BK84" s="38"/>
+      <c r="BG84" s="41"/>
+      <c r="BH84" s="41"/>
+      <c r="BI84" s="41"/>
+      <c r="BJ84" s="41"/>
+      <c r="BK84" s="41"/>
       <c r="BL84" s="38"/>
       <c r="BM84" s="38"/>
       <c r="BN84" s="38"/>
@@ -9119,12 +9147,10 @@
       <c r="BY84" s="38"/>
       <c r="BZ84" s="38"/>
     </row>
-    <row r="85" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A85" s="32"/>
       <c r="B85" s="53"/>
-      <c r="C85" s="56" t="s">
-        <v>98</v>
-      </c>
+      <c r="C85" s="56"/>
       <c r="D85" s="54"/>
       <c r="E85" s="35"/>
       <c r="F85" s="35"/>
@@ -9135,11 +9161,11 @@
       <c r="K85" s="38"/>
       <c r="L85" s="38"/>
       <c r="M85" s="38"/>
-      <c r="N85" s="38"/>
-      <c r="O85" s="38"/>
-      <c r="P85" s="38"/>
-      <c r="Q85" s="38"/>
-      <c r="R85" s="38"/>
+      <c r="N85" s="44"/>
+      <c r="O85" s="44"/>
+      <c r="P85" s="44"/>
+      <c r="Q85" s="44"/>
+      <c r="R85" s="44"/>
       <c r="S85" s="38"/>
       <c r="T85" s="38"/>
       <c r="U85" s="38"/>
@@ -9150,11 +9176,11 @@
       <c r="Z85" s="38"/>
       <c r="AA85" s="38"/>
       <c r="AB85" s="38"/>
-      <c r="AC85" s="38"/>
-      <c r="AD85" s="38"/>
-      <c r="AE85" s="38"/>
-      <c r="AF85" s="38"/>
-      <c r="AG85" s="38"/>
+      <c r="AC85" s="39"/>
+      <c r="AD85" s="39"/>
+      <c r="AE85" s="39"/>
+      <c r="AF85" s="39"/>
+      <c r="AG85" s="39"/>
       <c r="AH85" s="38"/>
       <c r="AI85" s="38"/>
       <c r="AJ85" s="38"/>
@@ -9165,11 +9191,11 @@
       <c r="AO85" s="38"/>
       <c r="AP85" s="38"/>
       <c r="AQ85" s="38"/>
-      <c r="AR85" s="38"/>
-      <c r="AS85" s="38"/>
-      <c r="AT85" s="38"/>
-      <c r="AU85" s="38"/>
-      <c r="AV85" s="38"/>
+      <c r="AR85" s="40"/>
+      <c r="AS85" s="40"/>
+      <c r="AT85" s="40"/>
+      <c r="AU85" s="40"/>
+      <c r="AV85" s="40"/>
       <c r="AW85" s="38"/>
       <c r="AX85" s="38"/>
       <c r="AY85" s="38"/>
@@ -9180,11 +9206,11 @@
       <c r="BD85" s="38"/>
       <c r="BE85" s="38"/>
       <c r="BF85" s="38"/>
-      <c r="BG85" s="38"/>
-      <c r="BH85" s="38"/>
-      <c r="BI85" s="38"/>
-      <c r="BJ85" s="38"/>
-      <c r="BK85" s="38"/>
+      <c r="BG85" s="41"/>
+      <c r="BH85" s="41"/>
+      <c r="BI85" s="41"/>
+      <c r="BJ85" s="41"/>
+      <c r="BK85" s="41"/>
       <c r="BL85" s="38"/>
       <c r="BM85" s="38"/>
       <c r="BN85" s="38"/>
@@ -9201,173 +9227,175 @@
       <c r="BY85" s="38"/>
       <c r="BZ85" s="38"/>
     </row>
-    <row r="86" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="32"/>
-      <c r="B86" s="53"/>
-      <c r="C86" s="56"/>
-      <c r="D86" s="54"/>
-      <c r="E86" s="35"/>
-      <c r="F86" s="35"/>
-      <c r="G86" s="36"/>
-      <c r="H86" s="37"/>
-      <c r="I86" s="42"/>
-      <c r="J86" s="43"/>
-      <c r="K86" s="38"/>
-      <c r="L86" s="38"/>
-      <c r="M86" s="38"/>
-      <c r="N86" s="38"/>
-      <c r="O86" s="38"/>
-      <c r="P86" s="38"/>
-      <c r="Q86" s="38"/>
-      <c r="R86" s="38"/>
-      <c r="S86" s="38"/>
-      <c r="T86" s="38"/>
-      <c r="U86" s="38"/>
-      <c r="V86" s="38"/>
-      <c r="W86" s="38"/>
-      <c r="X86" s="38"/>
-      <c r="Y86" s="38"/>
-      <c r="Z86" s="38"/>
-      <c r="AA86" s="38"/>
-      <c r="AB86" s="38"/>
-      <c r="AC86" s="38"/>
-      <c r="AD86" s="38"/>
-      <c r="AE86" s="38"/>
-      <c r="AF86" s="38"/>
-      <c r="AG86" s="38"/>
-      <c r="AH86" s="38"/>
-      <c r="AI86" s="38"/>
-      <c r="AJ86" s="38"/>
-      <c r="AK86" s="38"/>
-      <c r="AL86" s="38"/>
-      <c r="AM86" s="38"/>
-      <c r="AN86" s="38"/>
-      <c r="AO86" s="38"/>
-      <c r="AP86" s="38"/>
-      <c r="AQ86" s="38"/>
-      <c r="AR86" s="38"/>
-      <c r="AS86" s="38"/>
-      <c r="AT86" s="38"/>
-      <c r="AU86" s="38"/>
-      <c r="AV86" s="38"/>
-      <c r="AW86" s="38"/>
-      <c r="AX86" s="38"/>
-      <c r="AY86" s="38"/>
-      <c r="AZ86" s="38"/>
-      <c r="BA86" s="38"/>
-      <c r="BB86" s="38"/>
-      <c r="BC86" s="38"/>
-      <c r="BD86" s="38"/>
-      <c r="BE86" s="38"/>
-      <c r="BF86" s="38"/>
-      <c r="BG86" s="38"/>
-      <c r="BH86" s="38"/>
-      <c r="BI86" s="38"/>
-      <c r="BJ86" s="38"/>
-      <c r="BK86" s="38"/>
-      <c r="BL86" s="38"/>
-      <c r="BM86" s="38"/>
-      <c r="BN86" s="38"/>
-      <c r="BO86" s="38"/>
-      <c r="BP86" s="38"/>
-      <c r="BQ86" s="38"/>
-      <c r="BR86" s="38"/>
-      <c r="BS86" s="38"/>
-      <c r="BT86" s="38"/>
-      <c r="BU86" s="38"/>
-      <c r="BV86" s="38"/>
-      <c r="BW86" s="38"/>
-      <c r="BX86" s="38"/>
-      <c r="BY86" s="38"/>
-      <c r="BZ86" s="38"/>
+    <row r="86" spans="1:78" s="105" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="91"/>
+      <c r="B86" s="92"/>
+      <c r="C86" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="D86" s="94"/>
+      <c r="E86" s="95"/>
+      <c r="F86" s="95"/>
+      <c r="G86" s="96"/>
+      <c r="H86" s="97"/>
+      <c r="I86" s="98"/>
+      <c r="J86" s="99"/>
+      <c r="K86" s="100"/>
+      <c r="L86" s="100"/>
+      <c r="M86" s="100"/>
+      <c r="N86" s="101"/>
+      <c r="O86" s="101"/>
+      <c r="P86" s="101"/>
+      <c r="Q86" s="101"/>
+      <c r="R86" s="101"/>
+      <c r="S86" s="100"/>
+      <c r="T86" s="100"/>
+      <c r="U86" s="100"/>
+      <c r="V86" s="100"/>
+      <c r="W86" s="100"/>
+      <c r="X86" s="100"/>
+      <c r="Y86" s="100"/>
+      <c r="Z86" s="100"/>
+      <c r="AA86" s="100"/>
+      <c r="AB86" s="100"/>
+      <c r="AC86" s="102"/>
+      <c r="AD86" s="102"/>
+      <c r="AE86" s="102"/>
+      <c r="AF86" s="102"/>
+      <c r="AG86" s="102"/>
+      <c r="AH86" s="100"/>
+      <c r="AI86" s="100"/>
+      <c r="AJ86" s="100"/>
+      <c r="AK86" s="100"/>
+      <c r="AL86" s="100"/>
+      <c r="AM86" s="100"/>
+      <c r="AN86" s="100"/>
+      <c r="AO86" s="100"/>
+      <c r="AP86" s="100"/>
+      <c r="AQ86" s="100"/>
+      <c r="AR86" s="103"/>
+      <c r="AS86" s="103"/>
+      <c r="AT86" s="103"/>
+      <c r="AU86" s="103"/>
+      <c r="AV86" s="103"/>
+      <c r="AW86" s="100"/>
+      <c r="AX86" s="100"/>
+      <c r="AY86" s="100"/>
+      <c r="AZ86" s="100"/>
+      <c r="BA86" s="100"/>
+      <c r="BB86" s="100"/>
+      <c r="BC86" s="100"/>
+      <c r="BD86" s="100"/>
+      <c r="BE86" s="100"/>
+      <c r="BF86" s="100"/>
+      <c r="BG86" s="104"/>
+      <c r="BH86" s="104"/>
+      <c r="BI86" s="104"/>
+      <c r="BJ86" s="104"/>
+      <c r="BK86" s="104"/>
+      <c r="BL86" s="100"/>
+      <c r="BM86" s="100"/>
+      <c r="BN86" s="100"/>
+      <c r="BO86" s="100"/>
+      <c r="BP86" s="100"/>
+      <c r="BQ86" s="100"/>
+      <c r="BR86" s="100"/>
+      <c r="BS86" s="100"/>
+      <c r="BT86" s="100"/>
+      <c r="BU86" s="100"/>
+      <c r="BV86" s="100"/>
+      <c r="BW86" s="100"/>
+      <c r="BX86" s="100"/>
+      <c r="BY86" s="100"/>
+      <c r="BZ86" s="100"/>
     </row>
-    <row r="87" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="72"/>
-      <c r="B87" s="59"/>
-      <c r="C87" s="77" t="s">
-        <v>43</v>
-      </c>
-      <c r="D87" s="61"/>
-      <c r="E87" s="62"/>
-      <c r="F87" s="62"/>
-      <c r="G87" s="63"/>
-      <c r="H87" s="64"/>
-      <c r="I87" s="65"/>
-      <c r="J87" s="66"/>
-      <c r="K87" s="67"/>
-      <c r="L87" s="67"/>
-      <c r="M87" s="67"/>
-      <c r="N87" s="68"/>
-      <c r="O87" s="68"/>
-      <c r="P87" s="68"/>
-      <c r="Q87" s="68"/>
-      <c r="R87" s="68"/>
-      <c r="S87" s="67"/>
-      <c r="T87" s="67"/>
-      <c r="U87" s="67"/>
-      <c r="V87" s="67"/>
-      <c r="W87" s="67"/>
-      <c r="X87" s="67"/>
-      <c r="Y87" s="67"/>
-      <c r="Z87" s="67"/>
-      <c r="AA87" s="67"/>
-      <c r="AB87" s="67"/>
-      <c r="AC87" s="69"/>
-      <c r="AD87" s="69"/>
-      <c r="AE87" s="69"/>
-      <c r="AF87" s="69"/>
-      <c r="AG87" s="69"/>
-      <c r="AH87" s="67"/>
-      <c r="AI87" s="67"/>
-      <c r="AJ87" s="67"/>
-      <c r="AK87" s="67"/>
-      <c r="AL87" s="67"/>
-      <c r="AM87" s="67"/>
-      <c r="AN87" s="67"/>
-      <c r="AO87" s="67"/>
-      <c r="AP87" s="67"/>
-      <c r="AQ87" s="67"/>
-      <c r="AR87" s="70"/>
-      <c r="AS87" s="70"/>
-      <c r="AT87" s="70"/>
-      <c r="AU87" s="70"/>
-      <c r="AV87" s="70"/>
-      <c r="AW87" s="67"/>
-      <c r="AX87" s="67"/>
-      <c r="AY87" s="67"/>
-      <c r="AZ87" s="67"/>
-      <c r="BA87" s="67"/>
-      <c r="BB87" s="67"/>
-      <c r="BC87" s="67"/>
-      <c r="BD87" s="67"/>
-      <c r="BE87" s="67"/>
-      <c r="BF87" s="67"/>
-      <c r="BG87" s="71"/>
-      <c r="BH87" s="71"/>
-      <c r="BI87" s="71"/>
-      <c r="BJ87" s="71"/>
-      <c r="BK87" s="71"/>
-      <c r="BL87" s="67"/>
-      <c r="BM87" s="67"/>
-      <c r="BN87" s="67"/>
-      <c r="BO87" s="67"/>
-      <c r="BP87" s="67"/>
-      <c r="BQ87" s="67"/>
-      <c r="BR87" s="67"/>
-      <c r="BS87" s="67"/>
-      <c r="BT87" s="67"/>
-      <c r="BU87" s="67"/>
-      <c r="BV87" s="67"/>
-      <c r="BW87" s="67"/>
-      <c r="BX87" s="67"/>
-      <c r="BY87" s="67"/>
-      <c r="BZ87" s="67"/>
+    <row r="87" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="32"/>
+      <c r="B87" s="53"/>
+      <c r="C87" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="D87" s="54"/>
+      <c r="E87" s="35"/>
+      <c r="F87" s="35"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="37"/>
+      <c r="I87" s="42"/>
+      <c r="J87" s="43"/>
+      <c r="K87" s="38"/>
+      <c r="L87" s="38"/>
+      <c r="M87" s="38"/>
+      <c r="N87" s="38"/>
+      <c r="O87" s="38"/>
+      <c r="P87" s="38"/>
+      <c r="Q87" s="38"/>
+      <c r="R87" s="38"/>
+      <c r="S87" s="38"/>
+      <c r="T87" s="38"/>
+      <c r="U87" s="38"/>
+      <c r="V87" s="38"/>
+      <c r="W87" s="38"/>
+      <c r="X87" s="38"/>
+      <c r="Y87" s="38"/>
+      <c r="Z87" s="38"/>
+      <c r="AA87" s="38"/>
+      <c r="AB87" s="38"/>
+      <c r="AC87" s="38"/>
+      <c r="AD87" s="38"/>
+      <c r="AE87" s="38"/>
+      <c r="AF87" s="38"/>
+      <c r="AG87" s="38"/>
+      <c r="AH87" s="38"/>
+      <c r="AI87" s="124"/>
+      <c r="AJ87" s="124"/>
+      <c r="AK87" s="124"/>
+      <c r="AL87" s="124"/>
+      <c r="AM87" s="58"/>
+      <c r="AN87" s="38"/>
+      <c r="AO87" s="38"/>
+      <c r="AP87" s="38"/>
+      <c r="AQ87" s="38"/>
+      <c r="AR87" s="38"/>
+      <c r="AS87" s="38"/>
+      <c r="AT87" s="38"/>
+      <c r="AU87" s="38"/>
+      <c r="AV87" s="38"/>
+      <c r="AW87" s="38"/>
+      <c r="AX87" s="38"/>
+      <c r="AY87" s="38"/>
+      <c r="AZ87" s="38"/>
+      <c r="BA87" s="38"/>
+      <c r="BB87" s="38"/>
+      <c r="BC87" s="38"/>
+      <c r="BD87" s="38"/>
+      <c r="BE87" s="38"/>
+      <c r="BF87" s="38"/>
+      <c r="BG87" s="38"/>
+      <c r="BH87" s="38"/>
+      <c r="BI87" s="38"/>
+      <c r="BJ87" s="38"/>
+      <c r="BK87" s="38"/>
+      <c r="BL87" s="38"/>
+      <c r="BM87" s="38"/>
+      <c r="BN87" s="38"/>
+      <c r="BO87" s="38"/>
+      <c r="BP87" s="38"/>
+      <c r="BQ87" s="38"/>
+      <c r="BR87" s="38"/>
+      <c r="BS87" s="38"/>
+      <c r="BT87" s="38"/>
+      <c r="BU87" s="38"/>
+      <c r="BV87" s="38"/>
+      <c r="BW87" s="38"/>
+      <c r="BX87" s="38"/>
+      <c r="BY87" s="38"/>
+      <c r="BZ87" s="38"/>
     </row>
-    <row r="88" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A88" s="32"/>
       <c r="B88" s="53"/>
       <c r="C88" s="56" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D88" s="54"/>
       <c r="E88" s="35"/>
@@ -9379,11 +9407,11 @@
       <c r="K88" s="38"/>
       <c r="L88" s="38"/>
       <c r="M88" s="38"/>
-      <c r="N88" s="44"/>
-      <c r="O88" s="44"/>
-      <c r="P88" s="44"/>
-      <c r="Q88" s="44"/>
-      <c r="R88" s="44"/>
+      <c r="N88" s="38"/>
+      <c r="O88" s="38"/>
+      <c r="P88" s="38"/>
+      <c r="Q88" s="38"/>
+      <c r="R88" s="38"/>
       <c r="S88" s="38"/>
       <c r="T88" s="38"/>
       <c r="U88" s="38"/>
@@ -9394,26 +9422,26 @@
       <c r="Z88" s="38"/>
       <c r="AA88" s="38"/>
       <c r="AB88" s="38"/>
-      <c r="AC88" s="39"/>
-      <c r="AD88" s="39"/>
-      <c r="AE88" s="39"/>
-      <c r="AF88" s="39"/>
-      <c r="AG88" s="39"/>
-      <c r="AH88" s="124"/>
-      <c r="AI88" s="124"/>
-      <c r="AJ88" s="124"/>
-      <c r="AK88" s="124"/>
-      <c r="AL88" s="124"/>
-      <c r="AM88" s="58"/>
+      <c r="AC88" s="38"/>
+      <c r="AD88" s="38"/>
+      <c r="AE88" s="38"/>
+      <c r="AF88" s="38"/>
+      <c r="AG88" s="38"/>
+      <c r="AH88" s="38"/>
+      <c r="AI88" s="38"/>
+      <c r="AJ88" s="38"/>
+      <c r="AK88" s="38"/>
+      <c r="AL88" s="38"/>
+      <c r="AM88" s="38"/>
       <c r="AN88" s="38"/>
       <c r="AO88" s="38"/>
       <c r="AP88" s="38"/>
       <c r="AQ88" s="38"/>
-      <c r="AR88" s="40"/>
-      <c r="AS88" s="40"/>
-      <c r="AT88" s="40"/>
-      <c r="AU88" s="40"/>
-      <c r="AV88" s="40"/>
+      <c r="AR88" s="38"/>
+      <c r="AS88" s="38"/>
+      <c r="AT88" s="38"/>
+      <c r="AU88" s="38"/>
+      <c r="AV88" s="38"/>
       <c r="AW88" s="38"/>
       <c r="AX88" s="38"/>
       <c r="AY88" s="38"/>
@@ -9424,11 +9452,11 @@
       <c r="BD88" s="38"/>
       <c r="BE88" s="38"/>
       <c r="BF88" s="38"/>
-      <c r="BG88" s="41"/>
-      <c r="BH88" s="41"/>
-      <c r="BI88" s="41"/>
-      <c r="BJ88" s="41"/>
-      <c r="BK88" s="41"/>
+      <c r="BG88" s="38"/>
+      <c r="BH88" s="38"/>
+      <c r="BI88" s="38"/>
+      <c r="BJ88" s="38"/>
+      <c r="BK88" s="38"/>
       <c r="BL88" s="38"/>
       <c r="BM88" s="38"/>
       <c r="BN88" s="38"/>
@@ -9445,12 +9473,10 @@
       <c r="BY88" s="38"/>
       <c r="BZ88" s="38"/>
     </row>
-    <row r="89" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A89" s="32"/>
       <c r="B89" s="53"/>
-      <c r="C89" s="56" t="s">
-        <v>85</v>
-      </c>
+      <c r="C89" s="56"/>
       <c r="D89" s="54"/>
       <c r="E89" s="35"/>
       <c r="F89" s="35"/>
@@ -9461,11 +9487,11 @@
       <c r="K89" s="38"/>
       <c r="L89" s="38"/>
       <c r="M89" s="38"/>
-      <c r="N89" s="44"/>
-      <c r="O89" s="44"/>
-      <c r="P89" s="44"/>
-      <c r="Q89" s="44"/>
-      <c r="R89" s="44"/>
+      <c r="N89" s="38"/>
+      <c r="O89" s="38"/>
+      <c r="P89" s="38"/>
+      <c r="Q89" s="38"/>
+      <c r="R89" s="38"/>
       <c r="S89" s="38"/>
       <c r="T89" s="38"/>
       <c r="U89" s="38"/>
@@ -9476,26 +9502,26 @@
       <c r="Z89" s="38"/>
       <c r="AA89" s="38"/>
       <c r="AB89" s="38"/>
-      <c r="AC89" s="39"/>
-      <c r="AD89" s="39"/>
-      <c r="AE89" s="39"/>
-      <c r="AF89" s="39"/>
-      <c r="AG89" s="39"/>
-      <c r="AH89" s="124"/>
-      <c r="AI89" s="124"/>
-      <c r="AJ89" s="124"/>
-      <c r="AK89" s="124"/>
-      <c r="AL89" s="124"/>
-      <c r="AM89" s="58"/>
+      <c r="AC89" s="38"/>
+      <c r="AD89" s="38"/>
+      <c r="AE89" s="38"/>
+      <c r="AF89" s="38"/>
+      <c r="AG89" s="38"/>
+      <c r="AH89" s="38"/>
+      <c r="AI89" s="38"/>
+      <c r="AJ89" s="38"/>
+      <c r="AK89" s="38"/>
+      <c r="AL89" s="38"/>
+      <c r="AM89" s="38"/>
       <c r="AN89" s="38"/>
       <c r="AO89" s="38"/>
       <c r="AP89" s="38"/>
       <c r="AQ89" s="38"/>
-      <c r="AR89" s="40"/>
-      <c r="AS89" s="40"/>
-      <c r="AT89" s="40"/>
-      <c r="AU89" s="40"/>
-      <c r="AV89" s="40"/>
+      <c r="AR89" s="38"/>
+      <c r="AS89" s="38"/>
+      <c r="AT89" s="38"/>
+      <c r="AU89" s="38"/>
+      <c r="AV89" s="38"/>
       <c r="AW89" s="38"/>
       <c r="AX89" s="38"/>
       <c r="AY89" s="38"/>
@@ -9506,11 +9532,11 @@
       <c r="BD89" s="38"/>
       <c r="BE89" s="38"/>
       <c r="BF89" s="38"/>
-      <c r="BG89" s="41"/>
-      <c r="BH89" s="41"/>
-      <c r="BI89" s="41"/>
-      <c r="BJ89" s="41"/>
-      <c r="BK89" s="41"/>
+      <c r="BG89" s="38"/>
+      <c r="BH89" s="38"/>
+      <c r="BI89" s="38"/>
+      <c r="BJ89" s="38"/>
+      <c r="BK89" s="38"/>
       <c r="BL89" s="38"/>
       <c r="BM89" s="38"/>
       <c r="BN89" s="38"/>
@@ -9527,90 +9553,94 @@
       <c r="BY89" s="38"/>
       <c r="BZ89" s="38"/>
     </row>
-    <row r="90" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="32"/>
-      <c r="B90" s="53"/>
-      <c r="C90" s="56"/>
-      <c r="D90" s="54"/>
-      <c r="E90" s="35"/>
-      <c r="F90" s="35"/>
-      <c r="G90" s="36"/>
-      <c r="H90" s="37"/>
-      <c r="I90" s="42"/>
-      <c r="J90" s="43"/>
-      <c r="K90" s="38"/>
-      <c r="L90" s="38"/>
-      <c r="M90" s="38"/>
-      <c r="N90" s="44"/>
-      <c r="O90" s="44"/>
-      <c r="P90" s="44"/>
-      <c r="Q90" s="44"/>
-      <c r="R90" s="44"/>
-      <c r="S90" s="38"/>
-      <c r="T90" s="38"/>
-      <c r="U90" s="38"/>
-      <c r="V90" s="38"/>
-      <c r="W90" s="38"/>
-      <c r="X90" s="38"/>
-      <c r="Y90" s="38"/>
-      <c r="Z90" s="38"/>
-      <c r="AA90" s="38"/>
-      <c r="AB90" s="38"/>
-      <c r="AC90" s="39"/>
-      <c r="AD90" s="39"/>
-      <c r="AE90" s="39"/>
-      <c r="AF90" s="39"/>
-      <c r="AG90" s="39"/>
-      <c r="AH90" s="38"/>
-      <c r="AI90" s="38"/>
-      <c r="AJ90" s="38"/>
-      <c r="AK90" s="38"/>
-      <c r="AL90" s="38"/>
-      <c r="AM90" s="38"/>
-      <c r="AN90" s="38"/>
-      <c r="AO90" s="38"/>
-      <c r="AP90" s="38"/>
-      <c r="AQ90" s="38"/>
-      <c r="AR90" s="40"/>
-      <c r="AS90" s="40"/>
-      <c r="AT90" s="40"/>
-      <c r="AU90" s="40"/>
-      <c r="AV90" s="40"/>
-      <c r="AW90" s="38"/>
-      <c r="AX90" s="38"/>
-      <c r="AY90" s="38"/>
-      <c r="AZ90" s="38"/>
-      <c r="BA90" s="38"/>
-      <c r="BB90" s="38"/>
-      <c r="BC90" s="38"/>
-      <c r="BD90" s="38"/>
-      <c r="BE90" s="38"/>
-      <c r="BF90" s="38"/>
-      <c r="BG90" s="41"/>
-      <c r="BH90" s="41"/>
-      <c r="BI90" s="41"/>
-      <c r="BJ90" s="41"/>
-      <c r="BK90" s="41"/>
-      <c r="BL90" s="38"/>
-      <c r="BM90" s="38"/>
-      <c r="BN90" s="38"/>
-      <c r="BO90" s="38"/>
-      <c r="BP90" s="38"/>
-      <c r="BQ90" s="38"/>
-      <c r="BR90" s="38"/>
-      <c r="BS90" s="38"/>
-      <c r="BT90" s="38"/>
-      <c r="BU90" s="38"/>
-      <c r="BV90" s="38"/>
-      <c r="BW90" s="38"/>
-      <c r="BX90" s="38"/>
-      <c r="BY90" s="38"/>
-      <c r="BZ90" s="38"/>
+    <row r="90" spans="1:78" s="75" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A90" s="72"/>
+      <c r="B90" s="59"/>
+      <c r="C90" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="D90" s="61"/>
+      <c r="E90" s="62"/>
+      <c r="F90" s="62"/>
+      <c r="G90" s="63"/>
+      <c r="H90" s="64"/>
+      <c r="I90" s="65"/>
+      <c r="J90" s="66"/>
+      <c r="K90" s="67"/>
+      <c r="L90" s="67"/>
+      <c r="M90" s="67"/>
+      <c r="N90" s="68"/>
+      <c r="O90" s="68"/>
+      <c r="P90" s="68"/>
+      <c r="Q90" s="68"/>
+      <c r="R90" s="68"/>
+      <c r="S90" s="67"/>
+      <c r="T90" s="67"/>
+      <c r="U90" s="67"/>
+      <c r="V90" s="67"/>
+      <c r="W90" s="67"/>
+      <c r="X90" s="67"/>
+      <c r="Y90" s="67"/>
+      <c r="Z90" s="67"/>
+      <c r="AA90" s="67"/>
+      <c r="AB90" s="67"/>
+      <c r="AC90" s="69"/>
+      <c r="AD90" s="69"/>
+      <c r="AE90" s="69"/>
+      <c r="AF90" s="69"/>
+      <c r="AG90" s="69"/>
+      <c r="AH90" s="67"/>
+      <c r="AI90" s="67"/>
+      <c r="AJ90" s="67"/>
+      <c r="AK90" s="67"/>
+      <c r="AL90" s="67"/>
+      <c r="AM90" s="67"/>
+      <c r="AN90" s="67"/>
+      <c r="AO90" s="67"/>
+      <c r="AP90" s="67"/>
+      <c r="AQ90" s="67"/>
+      <c r="AR90" s="70"/>
+      <c r="AS90" s="70"/>
+      <c r="AT90" s="70"/>
+      <c r="AU90" s="70"/>
+      <c r="AV90" s="70"/>
+      <c r="AW90" s="67"/>
+      <c r="AX90" s="67"/>
+      <c r="AY90" s="67"/>
+      <c r="AZ90" s="67"/>
+      <c r="BA90" s="67"/>
+      <c r="BB90" s="67"/>
+      <c r="BC90" s="67"/>
+      <c r="BD90" s="67"/>
+      <c r="BE90" s="67"/>
+      <c r="BF90" s="67"/>
+      <c r="BG90" s="71"/>
+      <c r="BH90" s="71"/>
+      <c r="BI90" s="71"/>
+      <c r="BJ90" s="71"/>
+      <c r="BK90" s="71"/>
+      <c r="BL90" s="67"/>
+      <c r="BM90" s="67"/>
+      <c r="BN90" s="67"/>
+      <c r="BO90" s="67"/>
+      <c r="BP90" s="67"/>
+      <c r="BQ90" s="67"/>
+      <c r="BR90" s="67"/>
+      <c r="BS90" s="67"/>
+      <c r="BT90" s="67"/>
+      <c r="BU90" s="67"/>
+      <c r="BV90" s="67"/>
+      <c r="BW90" s="67"/>
+      <c r="BX90" s="67"/>
+      <c r="BY90" s="67"/>
+      <c r="BZ90" s="67"/>
     </row>
-    <row r="91" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A91" s="32"/>
       <c r="B91" s="53"/>
-      <c r="C91" s="56"/>
+      <c r="C91" s="56" t="s">
+        <v>84</v>
+      </c>
       <c r="D91" s="54"/>
       <c r="E91" s="35"/>
       <c r="F91" s="35"/>
@@ -9641,12 +9671,12 @@
       <c r="AE91" s="39"/>
       <c r="AF91" s="39"/>
       <c r="AG91" s="39"/>
-      <c r="AH91" s="38"/>
-      <c r="AI91" s="38"/>
-      <c r="AJ91" s="38"/>
-      <c r="AK91" s="38"/>
-      <c r="AL91" s="38"/>
-      <c r="AM91" s="38"/>
+      <c r="AH91" s="124"/>
+      <c r="AI91" s="124"/>
+      <c r="AJ91" s="124"/>
+      <c r="AK91" s="124"/>
+      <c r="AL91" s="124"/>
+      <c r="AM91" s="58"/>
       <c r="AN91" s="38"/>
       <c r="AO91" s="38"/>
       <c r="AP91" s="38"/>
@@ -9687,10 +9717,12 @@
       <c r="BY91" s="38"/>
       <c r="BZ91" s="38"/>
     </row>
-    <row r="92" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A92" s="32"/>
       <c r="B92" s="53"/>
-      <c r="C92" s="56"/>
+      <c r="C92" s="56" t="s">
+        <v>85</v>
+      </c>
       <c r="D92" s="54"/>
       <c r="E92" s="35"/>
       <c r="F92" s="35"/>
@@ -9721,12 +9753,12 @@
       <c r="AE92" s="39"/>
       <c r="AF92" s="39"/>
       <c r="AG92" s="39"/>
-      <c r="AH92" s="38"/>
-      <c r="AI92" s="38"/>
-      <c r="AJ92" s="38"/>
-      <c r="AK92" s="38"/>
-      <c r="AL92" s="38"/>
-      <c r="AM92" s="38"/>
+      <c r="AH92" s="124"/>
+      <c r="AI92" s="124"/>
+      <c r="AJ92" s="124"/>
+      <c r="AK92" s="124"/>
+      <c r="AL92" s="124"/>
+      <c r="AM92" s="58"/>
       <c r="AN92" s="38"/>
       <c r="AO92" s="38"/>
       <c r="AP92" s="38"/>
@@ -9767,7 +9799,7 @@
       <c r="BY92" s="38"/>
       <c r="BZ92" s="38"/>
     </row>
-    <row r="93" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A93" s="32"/>
       <c r="B93" s="53"/>
       <c r="C93" s="56"/>
@@ -9847,10 +9879,10 @@
       <c r="BY93" s="38"/>
       <c r="BZ93" s="38"/>
     </row>
-    <row r="94" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
       <c r="A94" s="32"/>
       <c r="B94" s="53"/>
-      <c r="C94" s="57"/>
+      <c r="C94" s="56"/>
       <c r="D94" s="54"/>
       <c r="E94" s="35"/>
       <c r="F94" s="35"/>
@@ -9927,112 +9959,95 @@
       <c r="BY94" s="38"/>
       <c r="BZ94" s="38"/>
     </row>
-    <row r="95" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="26">
-        <v>4</v>
-      </c>
-      <c r="C95" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="D95" s="28"/>
-      <c r="E95" s="28"/>
-      <c r="F95" s="28"/>
-      <c r="G95" s="28"/>
-      <c r="H95" s="28"/>
-      <c r="I95" s="29"/>
-      <c r="J95" s="30"/>
-      <c r="K95" s="31"/>
-      <c r="L95" s="31"/>
-      <c r="M95" s="29"/>
-      <c r="N95" s="29"/>
-      <c r="O95" s="29"/>
-      <c r="P95" s="29"/>
-      <c r="Q95" s="29"/>
-      <c r="R95" s="29"/>
-      <c r="S95" s="29"/>
-      <c r="T95" s="29"/>
-      <c r="U95" s="29"/>
-      <c r="V95" s="29"/>
-      <c r="W95" s="29"/>
-      <c r="X95" s="29"/>
-      <c r="Y95" s="29"/>
-      <c r="Z95" s="29"/>
-      <c r="AA95" s="29"/>
-      <c r="AB95" s="29"/>
-      <c r="AC95" s="29"/>
-      <c r="AD95" s="29"/>
-      <c r="AE95" s="29"/>
-      <c r="AF95" s="29"/>
-      <c r="AG95" s="29"/>
-      <c r="AH95" s="29"/>
-      <c r="AI95" s="29"/>
-      <c r="AJ95" s="29"/>
-      <c r="AK95" s="29"/>
-      <c r="AL95" s="29"/>
-      <c r="AM95" s="29"/>
-      <c r="AN95" s="29"/>
-      <c r="AO95" s="29"/>
-      <c r="AP95" s="29"/>
-      <c r="AQ95" s="29"/>
-      <c r="AR95" s="29"/>
-      <c r="AS95" s="29"/>
-      <c r="AT95" s="29"/>
-      <c r="AU95" s="29"/>
-      <c r="AV95" s="29"/>
-      <c r="AW95" s="29"/>
-      <c r="AX95" s="29"/>
-      <c r="AY95" s="29"/>
-      <c r="AZ95" s="29"/>
-      <c r="BA95" s="29"/>
-      <c r="BB95" s="29"/>
-      <c r="BC95" s="29"/>
-      <c r="BD95" s="29"/>
-      <c r="BE95" s="29"/>
-      <c r="BF95" s="29"/>
-      <c r="BG95" s="29"/>
-      <c r="BH95" s="29"/>
-      <c r="BI95" s="29"/>
-      <c r="BJ95" s="29"/>
-      <c r="BK95" s="29"/>
-      <c r="BL95" s="29"/>
-      <c r="BM95" s="29"/>
-      <c r="BN95" s="29"/>
-      <c r="BO95" s="29"/>
-      <c r="BP95" s="29"/>
-      <c r="BQ95" s="29"/>
-      <c r="BR95" s="29"/>
-      <c r="BS95" s="29"/>
-      <c r="BT95" s="29"/>
-      <c r="BU95" s="29"/>
-      <c r="BV95" s="29"/>
-      <c r="BW95" s="29"/>
-      <c r="BX95" s="29"/>
-      <c r="BY95" s="29"/>
-      <c r="BZ95" s="29"/>
+    <row r="95" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A95" s="32"/>
+      <c r="B95" s="53"/>
+      <c r="C95" s="56"/>
+      <c r="D95" s="54"/>
+      <c r="E95" s="35"/>
+      <c r="F95" s="35"/>
+      <c r="G95" s="36"/>
+      <c r="H95" s="37"/>
+      <c r="I95" s="42"/>
+      <c r="J95" s="43"/>
+      <c r="K95" s="38"/>
+      <c r="L95" s="38"/>
+      <c r="M95" s="38"/>
+      <c r="N95" s="44"/>
+      <c r="O95" s="44"/>
+      <c r="P95" s="44"/>
+      <c r="Q95" s="44"/>
+      <c r="R95" s="44"/>
+      <c r="S95" s="38"/>
+      <c r="T95" s="38"/>
+      <c r="U95" s="38"/>
+      <c r="V95" s="38"/>
+      <c r="W95" s="38"/>
+      <c r="X95" s="38"/>
+      <c r="Y95" s="38"/>
+      <c r="Z95" s="38"/>
+      <c r="AA95" s="38"/>
+      <c r="AB95" s="38"/>
+      <c r="AC95" s="39"/>
+      <c r="AD95" s="39"/>
+      <c r="AE95" s="39"/>
+      <c r="AF95" s="39"/>
+      <c r="AG95" s="39"/>
+      <c r="AH95" s="38"/>
+      <c r="AI95" s="38"/>
+      <c r="AJ95" s="38"/>
+      <c r="AK95" s="38"/>
+      <c r="AL95" s="38"/>
+      <c r="AM95" s="38"/>
+      <c r="AN95" s="38"/>
+      <c r="AO95" s="38"/>
+      <c r="AP95" s="38"/>
+      <c r="AQ95" s="38"/>
+      <c r="AR95" s="40"/>
+      <c r="AS95" s="40"/>
+      <c r="AT95" s="40"/>
+      <c r="AU95" s="40"/>
+      <c r="AV95" s="40"/>
+      <c r="AW95" s="38"/>
+      <c r="AX95" s="38"/>
+      <c r="AY95" s="38"/>
+      <c r="AZ95" s="38"/>
+      <c r="BA95" s="38"/>
+      <c r="BB95" s="38"/>
+      <c r="BC95" s="38"/>
+      <c r="BD95" s="38"/>
+      <c r="BE95" s="38"/>
+      <c r="BF95" s="38"/>
+      <c r="BG95" s="41"/>
+      <c r="BH95" s="41"/>
+      <c r="BI95" s="41"/>
+      <c r="BJ95" s="41"/>
+      <c r="BK95" s="41"/>
+      <c r="BL95" s="38"/>
+      <c r="BM95" s="38"/>
+      <c r="BN95" s="38"/>
+      <c r="BO95" s="38"/>
+      <c r="BP95" s="38"/>
+      <c r="BQ95" s="38"/>
+      <c r="BR95" s="38"/>
+      <c r="BS95" s="38"/>
+      <c r="BT95" s="38"/>
+      <c r="BU95" s="38"/>
+      <c r="BV95" s="38"/>
+      <c r="BW95" s="38"/>
+      <c r="BX95" s="38"/>
+      <c r="BY95" s="38"/>
+      <c r="BZ95" s="38"/>
     </row>
-    <row r="96" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="33">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C96" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="D96" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="E96" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="F96" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="G96" s="36" t="e">
-        <f>DAYS360(E96,F96)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H96" s="37">
-        <v>1</v>
-      </c>
+    <row r="96" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="32"/>
+      <c r="B96" s="53"/>
+      <c r="C96" s="56"/>
+      <c r="D96" s="54"/>
+      <c r="E96" s="35"/>
+      <c r="F96" s="35"/>
+      <c r="G96" s="36"/>
+      <c r="H96" s="37"/>
       <c r="I96" s="42"/>
       <c r="J96" s="43"/>
       <c r="K96" s="38"/>
@@ -10104,28 +10119,15 @@
       <c r="BY96" s="38"/>
       <c r="BZ96" s="38"/>
     </row>
-    <row r="97" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="33">
-        <v>4.2</v>
-      </c>
-      <c r="C97" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="D97" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="E97" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="F97" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="G97" s="36">
-        <v>0</v>
-      </c>
-      <c r="H97" s="37">
-        <v>1</v>
-      </c>
+    <row r="97" spans="1:78" ht="17.25" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.15">
+      <c r="A97" s="32"/>
+      <c r="B97" s="53"/>
+      <c r="C97" s="57"/>
+      <c r="D97" s="54"/>
+      <c r="E97" s="35"/>
+      <c r="F97" s="35"/>
+      <c r="G97" s="36"/>
+      <c r="H97" s="37"/>
       <c r="I97" s="42"/>
       <c r="J97" s="43"/>
       <c r="K97" s="38"/>
@@ -10197,121 +10199,110 @@
       <c r="BY97" s="38"/>
       <c r="BZ97" s="38"/>
     </row>
-    <row r="98" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="C98" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="D98" s="34" t="s">
+    <row r="98" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B98" s="26">
+        <v>4</v>
+      </c>
+      <c r="C98" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="D98" s="28"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="28"/>
+      <c r="G98" s="28"/>
+      <c r="H98" s="28"/>
+      <c r="I98" s="29"/>
+      <c r="J98" s="30"/>
+      <c r="K98" s="31"/>
+      <c r="L98" s="31"/>
+      <c r="M98" s="29"/>
+      <c r="N98" s="29"/>
+      <c r="O98" s="29"/>
+      <c r="P98" s="29"/>
+      <c r="Q98" s="29"/>
+      <c r="R98" s="29"/>
+      <c r="S98" s="29"/>
+      <c r="T98" s="29"/>
+      <c r="U98" s="29"/>
+      <c r="V98" s="29"/>
+      <c r="W98" s="29"/>
+      <c r="X98" s="29"/>
+      <c r="Y98" s="29"/>
+      <c r="Z98" s="29"/>
+      <c r="AA98" s="29"/>
+      <c r="AB98" s="29"/>
+      <c r="AC98" s="29"/>
+      <c r="AD98" s="29"/>
+      <c r="AE98" s="29"/>
+      <c r="AF98" s="29"/>
+      <c r="AG98" s="29"/>
+      <c r="AH98" s="29"/>
+      <c r="AI98" s="29"/>
+      <c r="AJ98" s="29"/>
+      <c r="AK98" s="29"/>
+      <c r="AL98" s="29"/>
+      <c r="AM98" s="29"/>
+      <c r="AN98" s="29"/>
+      <c r="AO98" s="29"/>
+      <c r="AP98" s="29"/>
+      <c r="AQ98" s="29"/>
+      <c r="AR98" s="29"/>
+      <c r="AS98" s="29"/>
+      <c r="AT98" s="29"/>
+      <c r="AU98" s="29"/>
+      <c r="AV98" s="29"/>
+      <c r="AW98" s="29"/>
+      <c r="AX98" s="29"/>
+      <c r="AY98" s="29"/>
+      <c r="AZ98" s="29"/>
+      <c r="BA98" s="29"/>
+      <c r="BB98" s="29"/>
+      <c r="BC98" s="29"/>
+      <c r="BD98" s="29"/>
+      <c r="BE98" s="29"/>
+      <c r="BF98" s="29"/>
+      <c r="BG98" s="29"/>
+      <c r="BH98" s="29"/>
+      <c r="BI98" s="29"/>
+      <c r="BJ98" s="29"/>
+      <c r="BK98" s="29"/>
+      <c r="BL98" s="29"/>
+      <c r="BM98" s="29"/>
+      <c r="BN98" s="29"/>
+      <c r="BO98" s="29"/>
+      <c r="BP98" s="29"/>
+      <c r="BQ98" s="29"/>
+      <c r="BR98" s="29"/>
+      <c r="BS98" s="29"/>
+      <c r="BT98" s="29"/>
+      <c r="BU98" s="29"/>
+      <c r="BV98" s="29"/>
+      <c r="BW98" s="29"/>
+      <c r="BX98" s="29"/>
+      <c r="BY98" s="29"/>
+      <c r="BZ98" s="29"/>
+    </row>
+    <row r="99" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B99" s="33">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C99" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D99" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="E98" s="35">
-        <v>44823</v>
-      </c>
-      <c r="F98" s="35">
-        <v>44823</v>
-      </c>
-      <c r="G98" s="36">
-        <f t="shared" ref="G98:G102" si="4">DAYS360(E98,F98)</f>
-        <v>0</v>
-      </c>
-      <c r="H98" s="37">
-        <v>1</v>
-      </c>
-      <c r="I98" s="42"/>
-      <c r="J98" s="43"/>
-      <c r="K98" s="38"/>
-      <c r="L98" s="38"/>
-      <c r="M98" s="38"/>
-      <c r="N98" s="44"/>
-      <c r="O98" s="44"/>
-      <c r="P98" s="44"/>
-      <c r="Q98" s="44"/>
-      <c r="R98" s="44"/>
-      <c r="S98" s="38"/>
-      <c r="T98" s="38"/>
-      <c r="U98" s="38"/>
-      <c r="V98" s="38"/>
-      <c r="W98" s="38"/>
-      <c r="X98" s="38"/>
-      <c r="Y98" s="38"/>
-      <c r="Z98" s="38"/>
-      <c r="AA98" s="38"/>
-      <c r="AB98" s="38"/>
-      <c r="AC98" s="39"/>
-      <c r="AD98" s="39"/>
-      <c r="AE98" s="39"/>
-      <c r="AF98" s="39"/>
-      <c r="AG98" s="39"/>
-      <c r="AH98" s="38"/>
-      <c r="AI98" s="38"/>
-      <c r="AJ98" s="38"/>
-      <c r="AK98" s="38"/>
-      <c r="AL98" s="38"/>
-      <c r="AM98" s="38"/>
-      <c r="AN98" s="38"/>
-      <c r="AO98" s="38"/>
-      <c r="AP98" s="38"/>
-      <c r="AQ98" s="38"/>
-      <c r="AR98" s="40"/>
-      <c r="AS98" s="40"/>
-      <c r="AT98" s="40"/>
-      <c r="AU98" s="40"/>
-      <c r="AV98" s="40"/>
-      <c r="AW98" s="38"/>
-      <c r="AX98" s="38"/>
-      <c r="AY98" s="38"/>
-      <c r="AZ98" s="38"/>
-      <c r="BA98" s="38"/>
-      <c r="BB98" s="38"/>
-      <c r="BC98" s="38"/>
-      <c r="BD98" s="38"/>
-      <c r="BE98" s="38"/>
-      <c r="BF98" s="38"/>
-      <c r="BG98" s="41"/>
-      <c r="BH98" s="41"/>
-      <c r="BI98" s="41"/>
-      <c r="BJ98" s="41"/>
-      <c r="BK98" s="41"/>
-      <c r="BL98" s="38"/>
-      <c r="BM98" s="38"/>
-      <c r="BN98" s="38"/>
-      <c r="BO98" s="38"/>
-      <c r="BP98" s="38"/>
-      <c r="BQ98" s="38"/>
-      <c r="BR98" s="38"/>
-      <c r="BS98" s="38"/>
-      <c r="BT98" s="38"/>
-      <c r="BU98" s="38"/>
-      <c r="BV98" s="38"/>
-      <c r="BW98" s="38"/>
-      <c r="BX98" s="38"/>
-      <c r="BY98" s="38"/>
-      <c r="BZ98" s="38"/>
-    </row>
-    <row r="99" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="C99" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="D99" s="34" t="s">
-        <v>55</v>
-      </c>
-      <c r="E99" s="35">
-        <v>44829</v>
-      </c>
-      <c r="F99" s="35">
-        <v>44829</v>
-      </c>
-      <c r="G99" s="36">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="H99" s="52">
+      <c r="E99" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="F99" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G99" s="36" t="e">
+        <f>DAYS360(E99,F99)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H99" s="37">
         <v>1</v>
       </c>
       <c r="I99" s="42"/>
@@ -10385,24 +10376,23 @@
       <c r="BY99" s="38"/>
       <c r="BZ99" s="38"/>
     </row>
-    <row r="100" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="33" t="s">
-        <v>53</v>
+    <row r="100" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B100" s="33">
+        <v>4.2</v>
       </c>
       <c r="C100" s="47" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D100" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="E100" s="35">
-        <v>44830</v>
-      </c>
-      <c r="F100" s="35">
-        <v>44830</v>
+      <c r="E100" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="F100" s="35" t="s">
+        <v>58</v>
       </c>
       <c r="G100" s="36">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H100" s="37">
@@ -10479,24 +10469,24 @@
       <c r="BY100" s="38"/>
       <c r="BZ100" s="38"/>
     </row>
-    <row r="101" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B101" s="33" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C101" s="47" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D101" s="34" t="s">
         <v>23</v>
       </c>
       <c r="E101" s="35">
-        <v>44837</v>
+        <v>44823</v>
       </c>
       <c r="F101" s="35">
-        <v>44837</v>
+        <v>44823</v>
       </c>
       <c r="G101" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="G101:G105" si="4">DAYS360(E101,F101)</f>
         <v>0</v>
       </c>
       <c r="H101" s="37">
@@ -10573,25 +10563,27 @@
       <c r="BY101" s="38"/>
       <c r="BZ101" s="38"/>
     </row>
-    <row r="102" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="33"/>
+    <row r="102" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B102" s="33" t="s">
+        <v>54</v>
+      </c>
       <c r="C102" s="47" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D102" s="34" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="E102" s="35">
-        <v>44844</v>
+        <v>44829</v>
       </c>
       <c r="F102" s="35">
-        <v>44844</v>
+        <v>44829</v>
       </c>
       <c r="G102" s="36">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H102" s="37">
+      <c r="H102" s="52">
         <v>1</v>
       </c>
       <c r="I102" s="42"/>
@@ -10665,24 +10657,24 @@
       <c r="BY102" s="38"/>
       <c r="BZ102" s="38"/>
     </row>
-    <row r="103" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B103" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C103" s="106" t="s">
-        <v>99</v>
+        <v>53</v>
+      </c>
+      <c r="C103" s="47" t="s">
+        <v>66</v>
       </c>
       <c r="D103" s="34" t="s">
         <v>23</v>
       </c>
       <c r="E103" s="35">
-        <v>44844</v>
+        <v>44830</v>
       </c>
       <c r="F103" s="35">
-        <v>44844</v>
+        <v>44830</v>
       </c>
       <c r="G103" s="36">
-        <f t="shared" ref="G103" si="5">DAYS360(E103,F103)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H103" s="37">
@@ -10759,87 +10751,387 @@
       <c r="BY103" s="38"/>
       <c r="BZ103" s="38"/>
     </row>
-    <row r="104" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="107"/>
-      <c r="C104" s="108"/>
-      <c r="D104" s="109"/>
-      <c r="E104" s="110"/>
-      <c r="F104" s="110"/>
-      <c r="G104" s="111"/>
-      <c r="H104" s="112"/>
-      <c r="I104" s="113"/>
-      <c r="J104" s="114"/>
-      <c r="K104" s="115"/>
-      <c r="L104" s="115"/>
-      <c r="M104" s="115"/>
-      <c r="N104" s="116"/>
-      <c r="O104" s="116"/>
-      <c r="P104" s="116"/>
-      <c r="Q104" s="116"/>
-      <c r="R104" s="116"/>
-      <c r="S104" s="115"/>
-      <c r="T104" s="115"/>
-      <c r="U104" s="115"/>
-      <c r="V104" s="115"/>
-      <c r="W104" s="115"/>
-      <c r="X104" s="115"/>
-      <c r="Y104" s="115"/>
-      <c r="Z104" s="115"/>
-      <c r="AA104" s="115"/>
-      <c r="AB104" s="115"/>
-      <c r="AC104" s="117"/>
-      <c r="AD104" s="117"/>
-      <c r="AE104" s="117"/>
-      <c r="AF104" s="117"/>
-      <c r="AG104" s="117"/>
-      <c r="AH104" s="115"/>
-      <c r="AI104" s="115"/>
-      <c r="AJ104" s="115"/>
-      <c r="AK104" s="115"/>
-      <c r="AL104" s="115"/>
-      <c r="AM104" s="115"/>
-      <c r="AN104" s="115"/>
-      <c r="AO104" s="115"/>
-      <c r="AP104" s="115"/>
-      <c r="AQ104" s="115"/>
-      <c r="AR104" s="118"/>
-      <c r="AS104" s="118"/>
-      <c r="AT104" s="118"/>
-      <c r="AU104" s="118"/>
-      <c r="AV104" s="118"/>
-      <c r="AW104" s="115"/>
-      <c r="AX104" s="115"/>
-      <c r="AY104" s="115"/>
-      <c r="AZ104" s="115"/>
-      <c r="BA104" s="115"/>
-      <c r="BB104" s="115"/>
-      <c r="BC104" s="115"/>
-      <c r="BD104" s="115"/>
-      <c r="BE104" s="115"/>
-      <c r="BF104" s="115"/>
-      <c r="BG104" s="119"/>
-      <c r="BH104" s="119"/>
-      <c r="BI104" s="119"/>
-      <c r="BJ104" s="119"/>
-      <c r="BK104" s="119"/>
-      <c r="BL104" s="115"/>
-      <c r="BM104" s="115"/>
-      <c r="BN104" s="115"/>
-      <c r="BO104" s="115"/>
-      <c r="BP104" s="115"/>
-      <c r="BQ104" s="115"/>
-      <c r="BR104" s="115"/>
-      <c r="BS104" s="115"/>
-      <c r="BT104" s="115"/>
-      <c r="BU104" s="115"/>
-      <c r="BV104" s="115"/>
-      <c r="BW104" s="115"/>
-      <c r="BX104" s="115"/>
-      <c r="BY104" s="115"/>
-      <c r="BZ104" s="115"/>
+    <row r="104" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B104" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C104" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D104" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E104" s="35">
+        <v>44837</v>
+      </c>
+      <c r="F104" s="35">
+        <v>44837</v>
+      </c>
+      <c r="G104" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H104" s="37">
+        <v>1</v>
+      </c>
+      <c r="I104" s="42"/>
+      <c r="J104" s="43"/>
+      <c r="K104" s="38"/>
+      <c r="L104" s="38"/>
+      <c r="M104" s="38"/>
+      <c r="N104" s="44"/>
+      <c r="O104" s="44"/>
+      <c r="P104" s="44"/>
+      <c r="Q104" s="44"/>
+      <c r="R104" s="44"/>
+      <c r="S104" s="38"/>
+      <c r="T104" s="38"/>
+      <c r="U104" s="38"/>
+      <c r="V104" s="38"/>
+      <c r="W104" s="38"/>
+      <c r="X104" s="38"/>
+      <c r="Y104" s="38"/>
+      <c r="Z104" s="38"/>
+      <c r="AA104" s="38"/>
+      <c r="AB104" s="38"/>
+      <c r="AC104" s="39"/>
+      <c r="AD104" s="39"/>
+      <c r="AE104" s="39"/>
+      <c r="AF104" s="39"/>
+      <c r="AG104" s="39"/>
+      <c r="AH104" s="38"/>
+      <c r="AI104" s="38"/>
+      <c r="AJ104" s="38"/>
+      <c r="AK104" s="38"/>
+      <c r="AL104" s="38"/>
+      <c r="AM104" s="38"/>
+      <c r="AN104" s="38"/>
+      <c r="AO104" s="38"/>
+      <c r="AP104" s="38"/>
+      <c r="AQ104" s="38"/>
+      <c r="AR104" s="40"/>
+      <c r="AS104" s="40"/>
+      <c r="AT104" s="40"/>
+      <c r="AU104" s="40"/>
+      <c r="AV104" s="40"/>
+      <c r="AW104" s="38"/>
+      <c r="AX104" s="38"/>
+      <c r="AY104" s="38"/>
+      <c r="AZ104" s="38"/>
+      <c r="BA104" s="38"/>
+      <c r="BB104" s="38"/>
+      <c r="BC104" s="38"/>
+      <c r="BD104" s="38"/>
+      <c r="BE104" s="38"/>
+      <c r="BF104" s="38"/>
+      <c r="BG104" s="41"/>
+      <c r="BH104" s="41"/>
+      <c r="BI104" s="41"/>
+      <c r="BJ104" s="41"/>
+      <c r="BK104" s="41"/>
+      <c r="BL104" s="38"/>
+      <c r="BM104" s="38"/>
+      <c r="BN104" s="38"/>
+      <c r="BO104" s="38"/>
+      <c r="BP104" s="38"/>
+      <c r="BQ104" s="38"/>
+      <c r="BR104" s="38"/>
+      <c r="BS104" s="38"/>
+      <c r="BT104" s="38"/>
+      <c r="BU104" s="38"/>
+      <c r="BV104" s="38"/>
+      <c r="BW104" s="38"/>
+      <c r="BX104" s="38"/>
+      <c r="BY104" s="38"/>
+      <c r="BZ104" s="38"/>
+    </row>
+    <row r="105" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B105" s="33"/>
+      <c r="C105" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="D105" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E105" s="35">
+        <v>44844</v>
+      </c>
+      <c r="F105" s="35">
+        <v>44844</v>
+      </c>
+      <c r="G105" s="36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H105" s="37">
+        <v>1</v>
+      </c>
+      <c r="I105" s="42"/>
+      <c r="J105" s="43"/>
+      <c r="K105" s="38"/>
+      <c r="L105" s="38"/>
+      <c r="M105" s="38"/>
+      <c r="N105" s="44"/>
+      <c r="O105" s="44"/>
+      <c r="P105" s="44"/>
+      <c r="Q105" s="44"/>
+      <c r="R105" s="44"/>
+      <c r="S105" s="38"/>
+      <c r="T105" s="38"/>
+      <c r="U105" s="38"/>
+      <c r="V105" s="38"/>
+      <c r="W105" s="38"/>
+      <c r="X105" s="38"/>
+      <c r="Y105" s="38"/>
+      <c r="Z105" s="38"/>
+      <c r="AA105" s="38"/>
+      <c r="AB105" s="38"/>
+      <c r="AC105" s="39"/>
+      <c r="AD105" s="39"/>
+      <c r="AE105" s="39"/>
+      <c r="AF105" s="39"/>
+      <c r="AG105" s="39"/>
+      <c r="AH105" s="38"/>
+      <c r="AI105" s="38"/>
+      <c r="AJ105" s="38"/>
+      <c r="AK105" s="38"/>
+      <c r="AL105" s="38"/>
+      <c r="AM105" s="38"/>
+      <c r="AN105" s="38"/>
+      <c r="AO105" s="38"/>
+      <c r="AP105" s="38"/>
+      <c r="AQ105" s="38"/>
+      <c r="AR105" s="40"/>
+      <c r="AS105" s="40"/>
+      <c r="AT105" s="40"/>
+      <c r="AU105" s="40"/>
+      <c r="AV105" s="40"/>
+      <c r="AW105" s="38"/>
+      <c r="AX105" s="38"/>
+      <c r="AY105" s="38"/>
+      <c r="AZ105" s="38"/>
+      <c r="BA105" s="38"/>
+      <c r="BB105" s="38"/>
+      <c r="BC105" s="38"/>
+      <c r="BD105" s="38"/>
+      <c r="BE105" s="38"/>
+      <c r="BF105" s="38"/>
+      <c r="BG105" s="41"/>
+      <c r="BH105" s="41"/>
+      <c r="BI105" s="41"/>
+      <c r="BJ105" s="41"/>
+      <c r="BK105" s="41"/>
+      <c r="BL105" s="38"/>
+      <c r="BM105" s="38"/>
+      <c r="BN105" s="38"/>
+      <c r="BO105" s="38"/>
+      <c r="BP105" s="38"/>
+      <c r="BQ105" s="38"/>
+      <c r="BR105" s="38"/>
+      <c r="BS105" s="38"/>
+      <c r="BT105" s="38"/>
+      <c r="BU105" s="38"/>
+      <c r="BV105" s="38"/>
+      <c r="BW105" s="38"/>
+      <c r="BX105" s="38"/>
+      <c r="BY105" s="38"/>
+      <c r="BZ105" s="38"/>
+    </row>
+    <row r="106" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B106" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C106" s="106" t="s">
+        <v>97</v>
+      </c>
+      <c r="D106" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E106" s="35">
+        <v>44844</v>
+      </c>
+      <c r="F106" s="35">
+        <v>44844</v>
+      </c>
+      <c r="G106" s="36">
+        <f t="shared" ref="G106" si="5">DAYS360(E106,F106)</f>
+        <v>0</v>
+      </c>
+      <c r="H106" s="37">
+        <v>1</v>
+      </c>
+      <c r="I106" s="42"/>
+      <c r="J106" s="43"/>
+      <c r="K106" s="38"/>
+      <c r="L106" s="38"/>
+      <c r="M106" s="38"/>
+      <c r="N106" s="44"/>
+      <c r="O106" s="44"/>
+      <c r="P106" s="44"/>
+      <c r="Q106" s="44"/>
+      <c r="R106" s="44"/>
+      <c r="S106" s="38"/>
+      <c r="T106" s="38"/>
+      <c r="U106" s="38"/>
+      <c r="V106" s="38"/>
+      <c r="W106" s="38"/>
+      <c r="X106" s="38"/>
+      <c r="Y106" s="38"/>
+      <c r="Z106" s="38"/>
+      <c r="AA106" s="38"/>
+      <c r="AB106" s="38"/>
+      <c r="AC106" s="39"/>
+      <c r="AD106" s="39"/>
+      <c r="AE106" s="39"/>
+      <c r="AF106" s="39"/>
+      <c r="AG106" s="39"/>
+      <c r="AH106" s="38"/>
+      <c r="AI106" s="38"/>
+      <c r="AJ106" s="38"/>
+      <c r="AK106" s="38"/>
+      <c r="AL106" s="38"/>
+      <c r="AM106" s="38"/>
+      <c r="AN106" s="38"/>
+      <c r="AO106" s="38"/>
+      <c r="AP106" s="38"/>
+      <c r="AQ106" s="38"/>
+      <c r="AR106" s="40"/>
+      <c r="AS106" s="40"/>
+      <c r="AT106" s="40"/>
+      <c r="AU106" s="40"/>
+      <c r="AV106" s="40"/>
+      <c r="AW106" s="38"/>
+      <c r="AX106" s="38"/>
+      <c r="AY106" s="38"/>
+      <c r="AZ106" s="38"/>
+      <c r="BA106" s="38"/>
+      <c r="BB106" s="38"/>
+      <c r="BC106" s="38"/>
+      <c r="BD106" s="38"/>
+      <c r="BE106" s="38"/>
+      <c r="BF106" s="38"/>
+      <c r="BG106" s="41"/>
+      <c r="BH106" s="41"/>
+      <c r="BI106" s="41"/>
+      <c r="BJ106" s="41"/>
+      <c r="BK106" s="41"/>
+      <c r="BL106" s="38"/>
+      <c r="BM106" s="38"/>
+      <c r="BN106" s="38"/>
+      <c r="BO106" s="38"/>
+      <c r="BP106" s="38"/>
+      <c r="BQ106" s="38"/>
+      <c r="BR106" s="38"/>
+      <c r="BS106" s="38"/>
+      <c r="BT106" s="38"/>
+      <c r="BU106" s="38"/>
+      <c r="BV106" s="38"/>
+      <c r="BW106" s="38"/>
+      <c r="BX106" s="38"/>
+      <c r="BY106" s="38"/>
+      <c r="BZ106" s="38"/>
+    </row>
+    <row r="107" spans="1:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B107" s="107"/>
+      <c r="C107" s="108"/>
+      <c r="D107" s="109"/>
+      <c r="E107" s="110"/>
+      <c r="F107" s="110"/>
+      <c r="G107" s="111"/>
+      <c r="H107" s="112"/>
+      <c r="I107" s="113"/>
+      <c r="J107" s="114"/>
+      <c r="K107" s="115"/>
+      <c r="L107" s="115"/>
+      <c r="M107" s="115"/>
+      <c r="N107" s="116"/>
+      <c r="O107" s="116"/>
+      <c r="P107" s="116"/>
+      <c r="Q107" s="116"/>
+      <c r="R107" s="116"/>
+      <c r="S107" s="115"/>
+      <c r="T107" s="115"/>
+      <c r="U107" s="115"/>
+      <c r="V107" s="115"/>
+      <c r="W107" s="115"/>
+      <c r="X107" s="115"/>
+      <c r="Y107" s="115"/>
+      <c r="Z107" s="115"/>
+      <c r="AA107" s="115"/>
+      <c r="AB107" s="115"/>
+      <c r="AC107" s="117"/>
+      <c r="AD107" s="117"/>
+      <c r="AE107" s="117"/>
+      <c r="AF107" s="117"/>
+      <c r="AG107" s="117"/>
+      <c r="AH107" s="115"/>
+      <c r="AI107" s="115"/>
+      <c r="AJ107" s="115"/>
+      <c r="AK107" s="115"/>
+      <c r="AL107" s="115"/>
+      <c r="AM107" s="115"/>
+      <c r="AN107" s="115"/>
+      <c r="AO107" s="115"/>
+      <c r="AP107" s="115"/>
+      <c r="AQ107" s="115"/>
+      <c r="AR107" s="118"/>
+      <c r="AS107" s="118"/>
+      <c r="AT107" s="118"/>
+      <c r="AU107" s="118"/>
+      <c r="AV107" s="118"/>
+      <c r="AW107" s="115"/>
+      <c r="AX107" s="115"/>
+      <c r="AY107" s="115"/>
+      <c r="AZ107" s="115"/>
+      <c r="BA107" s="115"/>
+      <c r="BB107" s="115"/>
+      <c r="BC107" s="115"/>
+      <c r="BD107" s="115"/>
+      <c r="BE107" s="115"/>
+      <c r="BF107" s="115"/>
+      <c r="BG107" s="119"/>
+      <c r="BH107" s="119"/>
+      <c r="BI107" s="119"/>
+      <c r="BJ107" s="119"/>
+      <c r="BK107" s="119"/>
+      <c r="BL107" s="115"/>
+      <c r="BM107" s="115"/>
+      <c r="BN107" s="115"/>
+      <c r="BO107" s="115"/>
+      <c r="BP107" s="115"/>
+      <c r="BQ107" s="115"/>
+      <c r="BR107" s="115"/>
+      <c r="BS107" s="115"/>
+      <c r="BT107" s="115"/>
+      <c r="BU107" s="115"/>
+      <c r="BV107" s="115"/>
+      <c r="BW107" s="115"/>
+      <c r="BX107" s="115"/>
+      <c r="BY107" s="115"/>
+      <c r="BZ107" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:AE2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="P4:AB4"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:W9"/>
+    <mergeCell ref="X9:AL9"/>
+    <mergeCell ref="AM9:BA9"/>
+    <mergeCell ref="X10:AB10"/>
+    <mergeCell ref="AC10:AG10"/>
+    <mergeCell ref="AH10:AL10"/>
+    <mergeCell ref="AM10:AQ10"/>
+    <mergeCell ref="AR10:AV10"/>
+    <mergeCell ref="AW10:BA10"/>
     <mergeCell ref="BB9:BZ9"/>
     <mergeCell ref="I10:M10"/>
     <mergeCell ref="N10:R10"/>
@@ -10856,29 +11148,9 @@
     <mergeCell ref="BQ10:BU10"/>
     <mergeCell ref="BV10:BZ10"/>
     <mergeCell ref="S10:W10"/>
-    <mergeCell ref="AM9:BA9"/>
-    <mergeCell ref="X10:AB10"/>
-    <mergeCell ref="AC10:AG10"/>
-    <mergeCell ref="AH10:AL10"/>
-    <mergeCell ref="AM10:AQ10"/>
-    <mergeCell ref="AR10:AV10"/>
-    <mergeCell ref="AW10:BA10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:AE2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="P4:AB4"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:W9"/>
-    <mergeCell ref="X9:AL9"/>
   </mergeCells>
   <phoneticPr fontId="35" type="noConversion"/>
-  <conditionalFormatting sqref="H12:H21 H23:H104">
+  <conditionalFormatting sqref="H12:H21 H23:H107">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -10888,7 +11160,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H21 H23:H104">
+  <conditionalFormatting sqref="H12:H21 H23:H107">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -10904,12 +11176,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F7EF2104F2CEFE4DACFBF5BA7D93FB4D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bb0ed258f694207805e211ca255f9b46">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6b71f768-6d8b-468c-a986-1e1afc74f0e3" xmlns:ns4="d07d918a-d172-4450-8f4a-7b087689ff85" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4c03c9fe975be0719773112499dde791" ns3:_="" ns4:_="">
     <xsd:import namespace="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
@@ -11138,6 +11404,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -11148,23 +11420,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6FABC364-430D-422C-AD85-145699D2125C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11183,6 +11438,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D564B3-5264-41FC-B8E0-395B567D9994}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="6b71f768-6d8b-468c-a986-1e1afc74f0e3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="d07d918a-d172-4450-8f4a-7b087689ff85"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7F187D4-7552-4664-8374-8AA9CBDA3C6B}">
   <ds:schemaRefs>

</xml_diff>